<commit_message>
update input file for DHW
</commit_message>
<xml_diff>
--- a/eureca_ubem/Input/Schedules.xlsx
+++ b/eureca_ubem/Input/Schedules.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20396"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20398"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pratenr82256\Desktop\eureca-ubem\eureca_ubem\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5A68787-7E07-4C93-A412-B072EC7B4EFD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D507CBBA-9830-4A3C-B8CD-C80371CC68AB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5580" yWindow="0" windowWidth="28800" windowHeight="12225" activeTab="1" xr2:uid="{102ADA3B-B81C-C94C-911C-48E8DF6FFDE7}"/>
+    <workbookView xWindow="8370" yWindow="0" windowWidth="28800" windowHeight="12225" activeTab="1" xr2:uid="{102ADA3B-B81C-C94C-911C-48E8DF6FFDE7}"/>
   </bookViews>
   <sheets>
     <sheet name="GeneralData" sheetId="10" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="42">
   <si>
     <t>Weekday</t>
   </si>
@@ -139,6 +139,21 @@
   <si>
     <t>Outdoor Air Ratio</t>
   </si>
+  <si>
+    <t>Domestic Hot Water FlowRate</t>
+  </si>
+  <si>
+    <t>[L/s]</t>
+  </si>
+  <si>
+    <t>DomesticHotWater calculation</t>
+  </si>
+  <si>
+    <t>[-]</t>
+  </si>
+  <si>
+    <t>UNI-TS 11300-2</t>
+  </si>
 </sst>
 </file>
 
@@ -156,7 +171,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -193,8 +208,38 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor rgb="FFA9D18E"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor rgb="FFC5E0B4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor rgb="FFA9D18E"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="25">
+  <borders count="32">
     <border>
       <left/>
       <right/>
@@ -534,11 +579,106 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -599,12 +739,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -615,6 +749,74 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -644,15 +846,6 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -674,13 +867,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
+      <xdr:col>11</xdr:col>
       <xdr:colOff>95250</xdr:colOff>
       <xdr:row>3</xdr:row>
       <xdr:rowOff>171450</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
+      <xdr:col>15</xdr:col>
       <xdr:colOff>581025</xdr:colOff>
       <xdr:row>9</xdr:row>
       <xdr:rowOff>171450</xdr:rowOff>
@@ -1047,10 +1240,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76CB4D20-8171-4D3A-B436-C3966BA8F7D8}">
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1061,34 +1254,38 @@
     <col min="4" max="4" width="13.375" customWidth="1"/>
     <col min="5" max="5" width="12.5" customWidth="1"/>
     <col min="6" max="6" width="12" customWidth="1"/>
-    <col min="8" max="8" width="14.375" customWidth="1"/>
+    <col min="7" max="7" width="17.5" customWidth="1"/>
+    <col min="10" max="10" width="14.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="20" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A1" s="26" t="s">
+    <row r="1" spans="1:10" s="20" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A1" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="27" t="s">
+      <c r="B1" s="47" t="s">
         <v>32</v>
       </c>
-      <c r="C1" s="27" t="s">
+      <c r="C1" s="25" t="s">
         <v>33</v>
       </c>
-      <c r="D1" s="27" t="s">
+      <c r="D1" s="25" t="s">
         <v>34</v>
       </c>
-      <c r="E1" s="27" t="s">
+      <c r="E1" s="25" t="s">
         <v>35</v>
       </c>
-      <c r="F1" s="27" t="s">
+      <c r="F1" s="25" t="s">
         <v>36</v>
       </c>
-      <c r="H1" s="20" t="s">
+      <c r="G1" s="49" t="s">
+        <v>39</v>
+      </c>
+      <c r="J1" s="20" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B2" s="14" t="s">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B2" s="48" t="s">
         <v>15</v>
       </c>
       <c r="C2" s="14" t="s">
@@ -1103,11 +1300,14 @@
       <c r="F2" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="H2" t="s">
+      <c r="G2" s="46" t="s">
+        <v>40</v>
+      </c>
+      <c r="J2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>22</v>
       </c>
@@ -1126,8 +1326,11 @@
       <c r="F3">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>23</v>
       </c>
@@ -1146,8 +1349,16 @@
       <c r="F4">
         <v>1</v>
       </c>
+      <c r="G4" t="s">
+        <v>20</v>
+      </c>
     </row>
   </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G3:G105" xr:uid="{8D8140ED-8C4A-489F-8C7E-0BC81CB30031}">
+      <formula1>"Schedule,UNI-TS 11300-2"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
@@ -1158,8 +1369,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE061425-C8E9-4A27-92D2-1582F4E407AA}">
   <dimension ref="A1:AS74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B29" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L72" sqref="L72"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="P51" sqref="P51:P74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1181,120 +1392,124 @@
       <c r="B1" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="C1" s="22" t="s">
-        <v>26</v>
-      </c>
-      <c r="D1" s="21" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" s="23" t="s">
+      <c r="C1" s="29" t="s">
+        <v>26</v>
+      </c>
+      <c r="D1" s="30" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="23" t="s">
+      <c r="F1" s="31" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="22" t="s">
+      <c r="G1" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="23" t="s">
+      <c r="H1" s="33" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="23" t="s">
+      <c r="I1" s="33" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="21" t="s">
+      <c r="J1" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="21" t="s">
+      <c r="K1" s="35" t="s">
         <v>4</v>
       </c>
-      <c r="L1" s="21" t="s">
+      <c r="L1" s="35" t="s">
         <v>28</v>
       </c>
-      <c r="M1" s="21" t="s">
+      <c r="M1" s="35" t="s">
         <v>29</v>
       </c>
-      <c r="N1" s="21" t="s">
+      <c r="N1" s="35" t="s">
         <v>30</v>
       </c>
-      <c r="O1" s="21" t="s">
+      <c r="O1" s="39" t="s">
         <v>31</v>
       </c>
-      <c r="P1" s="24"/>
-      <c r="Q1" s="24"/>
-      <c r="R1" s="24"/>
-      <c r="S1" s="24"/>
-      <c r="T1" s="24"/>
-      <c r="U1" s="24"/>
-      <c r="V1" s="24"/>
-      <c r="W1" s="24"/>
-      <c r="X1" s="24"/>
-      <c r="Y1" s="24"/>
-      <c r="Z1" s="24"/>
-      <c r="AA1" s="24"/>
-      <c r="AB1" s="24"/>
-      <c r="AC1" s="24"/>
-      <c r="AD1" s="24"/>
-      <c r="AE1" s="24"/>
-      <c r="AF1" s="24"/>
-      <c r="AG1" s="24"/>
-      <c r="AH1" s="25"/>
-      <c r="AI1" s="25"/>
-      <c r="AJ1" s="25"/>
-      <c r="AK1" s="25"/>
-      <c r="AL1" s="25"/>
-      <c r="AM1" s="25"/>
-      <c r="AN1" s="25"/>
-      <c r="AO1" s="25"/>
-      <c r="AP1" s="25"/>
-      <c r="AQ1" s="25"/>
-      <c r="AR1" s="25"/>
-      <c r="AS1" s="25"/>
+      <c r="P1" s="38" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q1" s="22"/>
+      <c r="R1" s="22"/>
+      <c r="S1" s="22"/>
+      <c r="T1" s="22"/>
+      <c r="U1" s="22"/>
+      <c r="V1" s="22"/>
+      <c r="W1" s="22"/>
+      <c r="X1" s="22"/>
+      <c r="Y1" s="22"/>
+      <c r="Z1" s="22"/>
+      <c r="AA1" s="22"/>
+      <c r="AB1" s="22"/>
+      <c r="AC1" s="22"/>
+      <c r="AD1" s="22"/>
+      <c r="AE1" s="22"/>
+      <c r="AF1" s="22"/>
+      <c r="AG1" s="22"/>
+      <c r="AH1" s="23"/>
+      <c r="AI1" s="23"/>
+      <c r="AJ1" s="23"/>
+      <c r="AK1" s="23"/>
+      <c r="AL1" s="23"/>
+      <c r="AM1" s="23"/>
+      <c r="AN1" s="23"/>
+      <c r="AO1" s="23"/>
+      <c r="AP1" s="23"/>
+      <c r="AQ1" s="23"/>
+      <c r="AR1" s="23"/>
+      <c r="AS1" s="23"/>
     </row>
     <row r="2" spans="1:45" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C2" s="37" t="s">
+      <c r="C2" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="38" t="s">
+      <c r="D2" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="38" t="s">
+      <c r="E2" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="38" t="s">
+      <c r="F2" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="G2" s="38" t="s">
+      <c r="G2" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="H2" s="38" t="s">
+      <c r="H2" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="I2" s="38" t="s">
+      <c r="I2" s="27" t="s">
         <v>13</v>
       </c>
-      <c r="J2" s="39" t="s">
+      <c r="J2" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="K2" s="38" t="s">
+      <c r="K2" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="L2" s="38" t="s">
+      <c r="L2" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="M2" s="38" t="s">
+      <c r="M2" s="27" t="s">
         <v>27</v>
       </c>
-      <c r="N2" s="38" t="s">
+      <c r="N2" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="O2" s="38" t="s">
+      <c r="O2" s="36" t="s">
         <v>27</v>
       </c>
-      <c r="P2" s="16"/>
+      <c r="P2" s="37" t="s">
+        <v>38</v>
+      </c>
       <c r="Q2" s="16"/>
       <c r="R2" s="16"/>
       <c r="S2" s="16"/>
@@ -1326,7 +1541,7 @@
       <c r="AS2" s="15"/>
     </row>
     <row r="3" spans="1:45" x14ac:dyDescent="0.25">
-      <c r="A3" s="28" t="s">
+      <c r="A3" s="50" t="s">
         <v>0</v>
       </c>
       <c r="B3" s="11">
@@ -1357,7 +1572,7 @@
         <v>60</v>
       </c>
       <c r="K3" s="2">
-        <v>0.2</v>
+        <v>8.0000000000000004E-4</v>
       </c>
       <c r="L3" s="2">
         <v>22</v>
@@ -1368,10 +1583,12 @@
       <c r="N3" s="2">
         <v>23</v>
       </c>
-      <c r="O3" s="6">
-        <v>1.0500000000000001E-2</v>
-      </c>
-      <c r="P3" s="15"/>
+      <c r="O3" s="40">
+        <v>1.0500000000000001E-2</v>
+      </c>
+      <c r="P3" s="43">
+        <v>0.01</v>
+      </c>
       <c r="Q3" s="15"/>
       <c r="R3" s="15"/>
       <c r="S3" s="15"/>
@@ -1403,7 +1620,7 @@
       <c r="AS3" s="15"/>
     </row>
     <row r="4" spans="1:45" x14ac:dyDescent="0.25">
-      <c r="A4" s="29"/>
+      <c r="A4" s="51"/>
       <c r="B4" s="12">
         <v>8.3333333333333301E-2</v>
       </c>
@@ -1432,7 +1649,7 @@
         <v>60</v>
       </c>
       <c r="K4" s="1">
-        <v>0.2</v>
+        <v>8.0000000000000004E-4</v>
       </c>
       <c r="L4" s="1">
         <v>22</v>
@@ -1443,10 +1660,12 @@
       <c r="N4" s="1">
         <v>23</v>
       </c>
-      <c r="O4" s="7">
+      <c r="O4" s="41">
         <v>1.15E-2</v>
       </c>
-      <c r="P4" s="15"/>
+      <c r="P4" s="44">
+        <v>0.01</v>
+      </c>
       <c r="Q4" s="15"/>
       <c r="R4" s="15"/>
       <c r="S4" s="15"/>
@@ -1478,7 +1697,7 @@
       <c r="AS4" s="15"/>
     </row>
     <row r="5" spans="1:45" x14ac:dyDescent="0.25">
-      <c r="A5" s="29"/>
+      <c r="A5" s="51"/>
       <c r="B5" s="12">
         <v>0.125</v>
       </c>
@@ -1507,7 +1726,7 @@
         <v>60</v>
       </c>
       <c r="K5" s="1">
-        <v>0.2</v>
+        <v>8.0000000000000004E-4</v>
       </c>
       <c r="L5" s="1">
         <v>22</v>
@@ -1518,10 +1737,12 @@
       <c r="N5" s="1">
         <v>23</v>
       </c>
-      <c r="O5" s="7">
+      <c r="O5" s="41">
         <v>1.15E-2</v>
       </c>
-      <c r="P5" s="15"/>
+      <c r="P5" s="44">
+        <v>0.01</v>
+      </c>
       <c r="Q5" s="15"/>
       <c r="R5" s="15"/>
       <c r="S5" s="15"/>
@@ -1553,7 +1774,7 @@
       <c r="AS5" s="15"/>
     </row>
     <row r="6" spans="1:45" x14ac:dyDescent="0.25">
-      <c r="A6" s="29"/>
+      <c r="A6" s="51"/>
       <c r="B6" s="12">
         <v>0.16666666666666699</v>
       </c>
@@ -1582,7 +1803,7 @@
         <v>60</v>
       </c>
       <c r="K6" s="1">
-        <v>0.2</v>
+        <v>8.0000000000000004E-4</v>
       </c>
       <c r="L6" s="1">
         <v>22</v>
@@ -1593,10 +1814,12 @@
       <c r="N6" s="1">
         <v>23</v>
       </c>
-      <c r="O6" s="7">
+      <c r="O6" s="41">
         <v>1.15E-2</v>
       </c>
-      <c r="P6" s="15"/>
+      <c r="P6" s="44">
+        <v>0.01</v>
+      </c>
       <c r="Q6" s="15"/>
       <c r="R6" s="15"/>
       <c r="S6" s="15"/>
@@ -1628,7 +1851,7 @@
       <c r="AS6" s="15"/>
     </row>
     <row r="7" spans="1:45" x14ac:dyDescent="0.25">
-      <c r="A7" s="29"/>
+      <c r="A7" s="51"/>
       <c r="B7" s="12">
         <v>0.20833333333333301</v>
       </c>
@@ -1657,7 +1880,7 @@
         <v>60</v>
       </c>
       <c r="K7" s="1">
-        <v>0.2</v>
+        <v>8.0000000000000004E-4</v>
       </c>
       <c r="L7" s="1">
         <v>22</v>
@@ -1668,10 +1891,12 @@
       <c r="N7" s="1">
         <v>23</v>
       </c>
-      <c r="O7" s="7">
+      <c r="O7" s="41">
         <v>1.15E-2</v>
       </c>
-      <c r="P7" s="15"/>
+      <c r="P7" s="44">
+        <v>0.01</v>
+      </c>
       <c r="Q7" s="15"/>
       <c r="R7" s="15"/>
       <c r="S7" s="15"/>
@@ -1703,7 +1928,7 @@
       <c r="AS7" s="15"/>
     </row>
     <row r="8" spans="1:45" x14ac:dyDescent="0.25">
-      <c r="A8" s="29"/>
+      <c r="A8" s="51"/>
       <c r="B8" s="12">
         <v>0.25</v>
       </c>
@@ -1732,7 +1957,7 @@
         <v>60</v>
       </c>
       <c r="K8" s="1">
-        <v>0.2</v>
+        <v>8.0000000000000004E-4</v>
       </c>
       <c r="L8" s="1">
         <v>22</v>
@@ -1743,10 +1968,12 @@
       <c r="N8" s="1">
         <v>23</v>
       </c>
-      <c r="O8" s="7">
+      <c r="O8" s="41">
         <v>1.15E-2</v>
       </c>
-      <c r="P8" s="15"/>
+      <c r="P8" s="44">
+        <v>0.01</v>
+      </c>
       <c r="Q8" s="15"/>
       <c r="R8" s="15"/>
       <c r="S8" s="15"/>
@@ -1778,7 +2005,7 @@
       <c r="AS8" s="15"/>
     </row>
     <row r="9" spans="1:45" x14ac:dyDescent="0.25">
-      <c r="A9" s="29"/>
+      <c r="A9" s="51"/>
       <c r="B9" s="12">
         <v>0.29166666666666702</v>
       </c>
@@ -1807,7 +2034,7 @@
         <v>60</v>
       </c>
       <c r="K9" s="1">
-        <v>0.2</v>
+        <v>8.0000000000000004E-4</v>
       </c>
       <c r="L9" s="1">
         <v>22</v>
@@ -1818,10 +2045,12 @@
       <c r="N9" s="1">
         <v>23</v>
       </c>
-      <c r="O9" s="7">
+      <c r="O9" s="41">
         <v>1.15E-2</v>
       </c>
-      <c r="P9" s="15"/>
+      <c r="P9" s="44">
+        <v>0.01</v>
+      </c>
       <c r="Q9" s="15"/>
       <c r="R9" s="15"/>
       <c r="S9" s="15"/>
@@ -1853,7 +2082,7 @@
       <c r="AS9" s="15"/>
     </row>
     <row r="10" spans="1:45" x14ac:dyDescent="0.25">
-      <c r="A10" s="29"/>
+      <c r="A10" s="51"/>
       <c r="B10" s="12">
         <v>0.33333333333333298</v>
       </c>
@@ -1882,7 +2111,7 @@
         <v>60</v>
       </c>
       <c r="K10" s="1">
-        <v>0.2</v>
+        <v>8.0000000000000004E-4</v>
       </c>
       <c r="L10" s="1">
         <v>22</v>
@@ -1893,10 +2122,12 @@
       <c r="N10" s="1">
         <v>23</v>
       </c>
-      <c r="O10" s="7">
+      <c r="O10" s="41">
         <v>1.15E-2</v>
       </c>
-      <c r="P10" s="15"/>
+      <c r="P10" s="44">
+        <v>0.03</v>
+      </c>
       <c r="Q10" s="15"/>
       <c r="R10" s="15"/>
       <c r="S10" s="15"/>
@@ -1928,7 +2159,7 @@
       <c r="AS10" s="15"/>
     </row>
     <row r="11" spans="1:45" x14ac:dyDescent="0.25">
-      <c r="A11" s="29"/>
+      <c r="A11" s="51"/>
       <c r="B11" s="12">
         <v>0.375</v>
       </c>
@@ -1957,7 +2188,7 @@
         <v>60</v>
       </c>
       <c r="K11" s="1">
-        <v>0.2</v>
+        <v>8.0000000000000004E-4</v>
       </c>
       <c r="L11" s="1">
         <v>22</v>
@@ -1968,12 +2199,15 @@
       <c r="N11" s="1">
         <v>23</v>
       </c>
-      <c r="O11" s="7">
+      <c r="O11" s="41">
         <v>1.15E-2</v>
       </c>
+      <c r="P11" s="44">
+        <v>0.03</v>
+      </c>
     </row>
     <row r="12" spans="1:45" x14ac:dyDescent="0.25">
-      <c r="A12" s="29"/>
+      <c r="A12" s="51"/>
       <c r="B12" s="12">
         <v>0.41666666666666702</v>
       </c>
@@ -2002,7 +2236,7 @@
         <v>60</v>
       </c>
       <c r="K12" s="1">
-        <v>0.2</v>
+        <v>8.0000000000000004E-4</v>
       </c>
       <c r="L12" s="1">
         <v>22</v>
@@ -2013,12 +2247,15 @@
       <c r="N12" s="1">
         <v>23</v>
       </c>
-      <c r="O12" s="7">
+      <c r="O12" s="41">
         <v>1.15E-2</v>
       </c>
+      <c r="P12" s="44">
+        <v>0.03</v>
+      </c>
     </row>
     <row r="13" spans="1:45" x14ac:dyDescent="0.25">
-      <c r="A13" s="29"/>
+      <c r="A13" s="51"/>
       <c r="B13" s="12">
         <v>0.45833333333333298</v>
       </c>
@@ -2047,7 +2284,7 @@
         <v>60</v>
       </c>
       <c r="K13" s="1">
-        <v>0.2</v>
+        <v>8.0000000000000004E-4</v>
       </c>
       <c r="L13" s="1">
         <v>22</v>
@@ -2058,12 +2295,15 @@
       <c r="N13" s="1">
         <v>23</v>
       </c>
-      <c r="O13" s="7">
+      <c r="O13" s="41">
         <v>1.15E-2</v>
       </c>
+      <c r="P13" s="44">
+        <v>0.03</v>
+      </c>
     </row>
     <row r="14" spans="1:45" x14ac:dyDescent="0.25">
-      <c r="A14" s="29"/>
+      <c r="A14" s="51"/>
       <c r="B14" s="12">
         <v>0.5</v>
       </c>
@@ -2092,7 +2332,7 @@
         <v>60</v>
       </c>
       <c r="K14" s="1">
-        <v>0.2</v>
+        <v>8.0000000000000004E-4</v>
       </c>
       <c r="L14" s="1">
         <v>22</v>
@@ -2103,12 +2343,15 @@
       <c r="N14" s="1">
         <v>23</v>
       </c>
-      <c r="O14" s="7">
+      <c r="O14" s="41">
         <v>1.15E-2</v>
       </c>
+      <c r="P14" s="44">
+        <v>0.03</v>
+      </c>
     </row>
     <row r="15" spans="1:45" x14ac:dyDescent="0.25">
-      <c r="A15" s="29"/>
+      <c r="A15" s="51"/>
       <c r="B15" s="12">
         <v>0.54166666666666696</v>
       </c>
@@ -2137,7 +2380,7 @@
         <v>60</v>
       </c>
       <c r="K15" s="1">
-        <v>0.2</v>
+        <v>8.0000000000000004E-4</v>
       </c>
       <c r="L15" s="1">
         <v>22</v>
@@ -2148,12 +2391,15 @@
       <c r="N15" s="1">
         <v>23</v>
       </c>
-      <c r="O15" s="7">
+      <c r="O15" s="41">
         <v>1.15E-2</v>
       </c>
+      <c r="P15" s="44">
+        <v>0.03</v>
+      </c>
     </row>
     <row r="16" spans="1:45" x14ac:dyDescent="0.25">
-      <c r="A16" s="29"/>
+      <c r="A16" s="51"/>
       <c r="B16" s="12">
         <v>0.58333333333333304</v>
       </c>
@@ -2182,7 +2428,7 @@
         <v>60</v>
       </c>
       <c r="K16" s="1">
-        <v>0.2</v>
+        <v>8.0000000000000004E-4</v>
       </c>
       <c r="L16" s="1">
         <v>22</v>
@@ -2193,12 +2439,15 @@
       <c r="N16" s="1">
         <v>23</v>
       </c>
-      <c r="O16" s="7">
+      <c r="O16" s="41">
         <v>1.15E-2</v>
       </c>
-    </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A17" s="29"/>
+      <c r="P16" s="44">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A17" s="51"/>
       <c r="B17" s="12">
         <v>0.625</v>
       </c>
@@ -2227,7 +2476,7 @@
         <v>60</v>
       </c>
       <c r="K17" s="1">
-        <v>0.2</v>
+        <v>8.0000000000000004E-4</v>
       </c>
       <c r="L17" s="1">
         <v>22</v>
@@ -2238,12 +2487,15 @@
       <c r="N17" s="1">
         <v>23</v>
       </c>
-      <c r="O17" s="7">
+      <c r="O17" s="41">
         <v>1.15E-2</v>
       </c>
-    </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A18" s="29"/>
+      <c r="P17" s="44">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A18" s="51"/>
       <c r="B18" s="12">
         <v>0.66666666666666696</v>
       </c>
@@ -2272,7 +2524,7 @@
         <v>60</v>
       </c>
       <c r="K18" s="1">
-        <v>0.2</v>
+        <v>8.0000000000000004E-4</v>
       </c>
       <c r="L18" s="1">
         <v>22</v>
@@ -2283,12 +2535,15 @@
       <c r="N18" s="1">
         <v>23</v>
       </c>
-      <c r="O18" s="7">
+      <c r="O18" s="41">
         <v>1.15E-2</v>
       </c>
-    </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A19" s="29"/>
+      <c r="P18" s="44">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A19" s="51"/>
       <c r="B19" s="12">
         <v>0.70833333333333304</v>
       </c>
@@ -2317,7 +2572,7 @@
         <v>60</v>
       </c>
       <c r="K19" s="1">
-        <v>0.2</v>
+        <v>8.0000000000000004E-4</v>
       </c>
       <c r="L19" s="1">
         <v>22</v>
@@ -2328,12 +2583,15 @@
       <c r="N19" s="1">
         <v>23</v>
       </c>
-      <c r="O19" s="7">
+      <c r="O19" s="41">
         <v>1.15E-2</v>
       </c>
-    </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A20" s="29"/>
+      <c r="P19" s="44">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A20" s="51"/>
       <c r="B20" s="12">
         <v>0.75</v>
       </c>
@@ -2362,7 +2620,7 @@
         <v>60</v>
       </c>
       <c r="K20" s="1">
-        <v>0.2</v>
+        <v>8.0000000000000004E-4</v>
       </c>
       <c r="L20" s="1">
         <v>22</v>
@@ -2373,12 +2631,15 @@
       <c r="N20" s="1">
         <v>23</v>
       </c>
-      <c r="O20" s="7">
+      <c r="O20" s="41">
         <v>1.15E-2</v>
       </c>
-    </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A21" s="29"/>
+      <c r="P20" s="44">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A21" s="51"/>
       <c r="B21" s="12">
         <v>0.79166666666666696</v>
       </c>
@@ -2407,7 +2668,7 @@
         <v>60</v>
       </c>
       <c r="K21" s="1">
-        <v>0.2</v>
+        <v>8.0000000000000004E-4</v>
       </c>
       <c r="L21" s="1">
         <v>22</v>
@@ -2418,12 +2679,15 @@
       <c r="N21" s="1">
         <v>23</v>
       </c>
-      <c r="O21" s="7">
+      <c r="O21" s="41">
         <v>1.15E-2</v>
       </c>
-    </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A22" s="29"/>
+      <c r="P21" s="44">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A22" s="51"/>
       <c r="B22" s="12">
         <v>0.83333333333333304</v>
       </c>
@@ -2452,7 +2716,7 @@
         <v>60</v>
       </c>
       <c r="K22" s="1">
-        <v>0.2</v>
+        <v>8.0000000000000004E-4</v>
       </c>
       <c r="L22" s="1">
         <v>22</v>
@@ -2463,12 +2727,15 @@
       <c r="N22" s="1">
         <v>23</v>
       </c>
-      <c r="O22" s="7">
+      <c r="O22" s="41">
         <v>1.15E-2</v>
       </c>
-    </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A23" s="29"/>
+      <c r="P22" s="44">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A23" s="51"/>
       <c r="B23" s="12">
         <v>0.875</v>
       </c>
@@ -2497,7 +2764,7 @@
         <v>60</v>
       </c>
       <c r="K23" s="1">
-        <v>0.2</v>
+        <v>8.0000000000000004E-4</v>
       </c>
       <c r="L23" s="1">
         <v>22</v>
@@ -2508,12 +2775,15 @@
       <c r="N23" s="1">
         <v>23</v>
       </c>
-      <c r="O23" s="7">
+      <c r="O23" s="41">
         <v>1.15E-2</v>
       </c>
-    </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A24" s="29"/>
+      <c r="P23" s="44">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A24" s="51"/>
       <c r="B24" s="12">
         <v>0.91666666666666696</v>
       </c>
@@ -2542,7 +2812,7 @@
         <v>60</v>
       </c>
       <c r="K24" s="1">
-        <v>0.2</v>
+        <v>8.0000000000000004E-4</v>
       </c>
       <c r="L24" s="1">
         <v>22</v>
@@ -2553,12 +2823,15 @@
       <c r="N24" s="1">
         <v>23</v>
       </c>
-      <c r="O24" s="7">
+      <c r="O24" s="41">
         <v>1.15E-2</v>
       </c>
-    </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A25" s="29"/>
+      <c r="P24" s="44">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A25" s="51"/>
       <c r="B25" s="12">
         <v>0.95833333333333304</v>
       </c>
@@ -2587,7 +2860,7 @@
         <v>60</v>
       </c>
       <c r="K25" s="1">
-        <v>0.2</v>
+        <v>8.0000000000000004E-4</v>
       </c>
       <c r="L25" s="1">
         <v>22</v>
@@ -2598,12 +2871,15 @@
       <c r="N25" s="1">
         <v>23</v>
       </c>
-      <c r="O25" s="7">
+      <c r="O25" s="41">
         <v>1.15E-2</v>
       </c>
-    </row>
-    <row r="26" spans="1:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="30"/>
+      <c r="P25" s="44">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="52"/>
       <c r="B26" s="13">
         <v>0.999999999999999</v>
       </c>
@@ -2632,7 +2908,7 @@
         <v>60</v>
       </c>
       <c r="K26" s="9">
-        <v>0.2</v>
+        <v>8.0000000000000004E-4</v>
       </c>
       <c r="L26" s="9">
         <v>22</v>
@@ -2643,12 +2919,15 @@
       <c r="N26" s="9">
         <v>23</v>
       </c>
-      <c r="O26" s="10">
+      <c r="O26" s="42">
         <v>1.15E-2</v>
       </c>
-    </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A27" s="31" t="s">
+      <c r="P26" s="45">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A27" s="53" t="s">
         <v>18</v>
       </c>
       <c r="B27" s="11">
@@ -2682,7 +2961,7 @@
         <v>60</v>
       </c>
       <c r="K27" s="2">
-        <v>0.2</v>
+        <v>8.0000000000000004E-4</v>
       </c>
       <c r="L27" s="2">
         <v>22</v>
@@ -2693,12 +2972,15 @@
       <c r="N27" s="2">
         <v>23</v>
       </c>
-      <c r="O27" s="6">
+      <c r="O27" s="40">
         <v>1.15E-2</v>
       </c>
-    </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A28" s="32"/>
+      <c r="P27" s="43">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A28" s="54"/>
       <c r="B28" s="12">
         <v>8.3333333333333301E-2</v>
       </c>
@@ -2730,7 +3012,7 @@
         <v>60</v>
       </c>
       <c r="K28" s="1">
-        <v>0.2</v>
+        <v>8.0000000000000004E-4</v>
       </c>
       <c r="L28" s="1">
         <v>22</v>
@@ -2741,12 +3023,15 @@
       <c r="N28" s="1">
         <v>23</v>
       </c>
-      <c r="O28" s="7">
+      <c r="O28" s="41">
         <v>1.15E-2</v>
       </c>
-    </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A29" s="32"/>
+      <c r="P28" s="44">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A29" s="54"/>
       <c r="B29" s="12">
         <v>0.125</v>
       </c>
@@ -2778,7 +3063,7 @@
         <v>60</v>
       </c>
       <c r="K29" s="1">
-        <v>0.2</v>
+        <v>8.0000000000000004E-4</v>
       </c>
       <c r="L29" s="1">
         <v>22</v>
@@ -2789,12 +3074,15 @@
       <c r="N29" s="1">
         <v>23</v>
       </c>
-      <c r="O29" s="7">
+      <c r="O29" s="41">
         <v>1.15E-2</v>
       </c>
-    </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A30" s="32"/>
+      <c r="P29" s="44">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A30" s="54"/>
       <c r="B30" s="12">
         <v>0.16666666666666699</v>
       </c>
@@ -2826,7 +3114,7 @@
         <v>60</v>
       </c>
       <c r="K30" s="1">
-        <v>0.2</v>
+        <v>8.0000000000000004E-4</v>
       </c>
       <c r="L30" s="1">
         <v>22</v>
@@ -2837,12 +3125,15 @@
       <c r="N30" s="1">
         <v>23</v>
       </c>
-      <c r="O30" s="7">
+      <c r="O30" s="41">
         <v>1.15E-2</v>
       </c>
-    </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A31" s="32"/>
+      <c r="P30" s="44">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A31" s="54"/>
       <c r="B31" s="12">
         <v>0.20833333333333301</v>
       </c>
@@ -2874,7 +3165,7 @@
         <v>60</v>
       </c>
       <c r="K31" s="1">
-        <v>0.2</v>
+        <v>8.0000000000000004E-4</v>
       </c>
       <c r="L31" s="1">
         <v>22</v>
@@ -2885,12 +3176,15 @@
       <c r="N31" s="1">
         <v>23</v>
       </c>
-      <c r="O31" s="7">
+      <c r="O31" s="41">
         <v>1.15E-2</v>
       </c>
-    </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A32" s="32"/>
+      <c r="P31" s="44">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A32" s="54"/>
       <c r="B32" s="12">
         <v>0.25</v>
       </c>
@@ -2922,7 +3216,7 @@
         <v>60</v>
       </c>
       <c r="K32" s="1">
-        <v>0.2</v>
+        <v>8.0000000000000004E-4</v>
       </c>
       <c r="L32" s="1">
         <v>22</v>
@@ -2933,12 +3227,15 @@
       <c r="N32" s="1">
         <v>23</v>
       </c>
-      <c r="O32" s="7">
+      <c r="O32" s="41">
         <v>1.15E-2</v>
       </c>
-    </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A33" s="32"/>
+      <c r="P32" s="44">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A33" s="54"/>
       <c r="B33" s="12">
         <v>0.29166666666666702</v>
       </c>
@@ -2970,7 +3267,7 @@
         <v>60</v>
       </c>
       <c r="K33" s="1">
-        <v>0.2</v>
+        <v>8.0000000000000004E-4</v>
       </c>
       <c r="L33" s="1">
         <v>22</v>
@@ -2981,12 +3278,15 @@
       <c r="N33" s="1">
         <v>23</v>
       </c>
-      <c r="O33" s="7">
+      <c r="O33" s="41">
         <v>1.15E-2</v>
       </c>
-    </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A34" s="32"/>
+      <c r="P33" s="44">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A34" s="54"/>
       <c r="B34" s="12">
         <v>0.33333333333333298</v>
       </c>
@@ -3018,7 +3318,7 @@
         <v>60</v>
       </c>
       <c r="K34" s="1">
-        <v>0.2</v>
+        <v>8.0000000000000004E-4</v>
       </c>
       <c r="L34" s="1">
         <v>22</v>
@@ -3029,12 +3329,15 @@
       <c r="N34" s="1">
         <v>23</v>
       </c>
-      <c r="O34" s="7">
+      <c r="O34" s="41">
         <v>1.15E-2</v>
       </c>
-    </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A35" s="32"/>
+      <c r="P34" s="44">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A35" s="54"/>
       <c r="B35" s="12">
         <v>0.375</v>
       </c>
@@ -3066,7 +3369,7 @@
         <v>60</v>
       </c>
       <c r="K35" s="1">
-        <v>0.2</v>
+        <v>8.0000000000000004E-4</v>
       </c>
       <c r="L35" s="1">
         <v>22</v>
@@ -3077,12 +3380,15 @@
       <c r="N35" s="1">
         <v>23</v>
       </c>
-      <c r="O35" s="7">
+      <c r="O35" s="41">
         <v>1.15E-2</v>
       </c>
-    </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A36" s="32"/>
+      <c r="P35" s="44">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A36" s="54"/>
       <c r="B36" s="12">
         <v>0.41666666666666702</v>
       </c>
@@ -3114,7 +3420,7 @@
         <v>60</v>
       </c>
       <c r="K36" s="1">
-        <v>0.2</v>
+        <v>8.0000000000000004E-4</v>
       </c>
       <c r="L36" s="1">
         <v>22</v>
@@ -3125,12 +3431,15 @@
       <c r="N36" s="1">
         <v>23</v>
       </c>
-      <c r="O36" s="7">
+      <c r="O36" s="41">
         <v>1.15E-2</v>
       </c>
-    </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A37" s="32"/>
+      <c r="P36" s="44">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A37" s="54"/>
       <c r="B37" s="12">
         <v>0.45833333333333298</v>
       </c>
@@ -3162,7 +3471,7 @@
         <v>60</v>
       </c>
       <c r="K37" s="1">
-        <v>0.2</v>
+        <v>8.0000000000000004E-4</v>
       </c>
       <c r="L37" s="1">
         <v>22</v>
@@ -3173,12 +3482,15 @@
       <c r="N37" s="1">
         <v>23</v>
       </c>
-      <c r="O37" s="7">
+      <c r="O37" s="41">
         <v>1.15E-2</v>
       </c>
-    </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A38" s="32"/>
+      <c r="P37" s="44">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A38" s="54"/>
       <c r="B38" s="12">
         <v>0.5</v>
       </c>
@@ -3210,7 +3522,7 @@
         <v>60</v>
       </c>
       <c r="K38" s="1">
-        <v>0.2</v>
+        <v>8.0000000000000004E-4</v>
       </c>
       <c r="L38" s="1">
         <v>22</v>
@@ -3221,12 +3533,15 @@
       <c r="N38" s="1">
         <v>23</v>
       </c>
-      <c r="O38" s="7">
+      <c r="O38" s="41">
         <v>1.15E-2</v>
       </c>
-    </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A39" s="32"/>
+      <c r="P38" s="44">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A39" s="54"/>
       <c r="B39" s="12">
         <v>0.54166666666666696</v>
       </c>
@@ -3258,7 +3573,7 @@
         <v>60</v>
       </c>
       <c r="K39" s="1">
-        <v>0.2</v>
+        <v>8.0000000000000004E-4</v>
       </c>
       <c r="L39" s="1">
         <v>22</v>
@@ -3269,12 +3584,15 @@
       <c r="N39" s="1">
         <v>23</v>
       </c>
-      <c r="O39" s="7">
+      <c r="O39" s="41">
         <v>1.15E-2</v>
       </c>
-    </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A40" s="32"/>
+      <c r="P39" s="44">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A40" s="54"/>
       <c r="B40" s="12">
         <v>0.58333333333333304</v>
       </c>
@@ -3306,7 +3624,7 @@
         <v>60</v>
       </c>
       <c r="K40" s="1">
-        <v>0.2</v>
+        <v>8.0000000000000004E-4</v>
       </c>
       <c r="L40" s="1">
         <v>22</v>
@@ -3317,12 +3635,15 @@
       <c r="N40" s="1">
         <v>23</v>
       </c>
-      <c r="O40" s="7">
+      <c r="O40" s="41">
         <v>1.15E-2</v>
       </c>
-    </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A41" s="32"/>
+      <c r="P40" s="44">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A41" s="54"/>
       <c r="B41" s="12">
         <v>0.625</v>
       </c>
@@ -3354,7 +3675,7 @@
         <v>60</v>
       </c>
       <c r="K41" s="1">
-        <v>0.2</v>
+        <v>8.0000000000000004E-4</v>
       </c>
       <c r="L41" s="1">
         <v>22</v>
@@ -3365,12 +3686,15 @@
       <c r="N41" s="1">
         <v>23</v>
       </c>
-      <c r="O41" s="7">
+      <c r="O41" s="41">
         <v>1.15E-2</v>
       </c>
-    </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A42" s="32"/>
+      <c r="P41" s="44">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A42" s="54"/>
       <c r="B42" s="12">
         <v>0.66666666666666696</v>
       </c>
@@ -3402,7 +3726,7 @@
         <v>60</v>
       </c>
       <c r="K42" s="1">
-        <v>0.2</v>
+        <v>8.0000000000000004E-4</v>
       </c>
       <c r="L42" s="1">
         <v>22</v>
@@ -3413,12 +3737,15 @@
       <c r="N42" s="1">
         <v>23</v>
       </c>
-      <c r="O42" s="7">
+      <c r="O42" s="41">
         <v>1.15E-2</v>
       </c>
-    </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A43" s="32"/>
+      <c r="P42" s="44">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A43" s="54"/>
       <c r="B43" s="12">
         <v>0.70833333333333304</v>
       </c>
@@ -3450,7 +3777,7 @@
         <v>60</v>
       </c>
       <c r="K43" s="1">
-        <v>0.2</v>
+        <v>8.0000000000000004E-4</v>
       </c>
       <c r="L43" s="1">
         <v>22</v>
@@ -3461,12 +3788,15 @@
       <c r="N43" s="1">
         <v>23</v>
       </c>
-      <c r="O43" s="7">
+      <c r="O43" s="41">
         <v>1.15E-2</v>
       </c>
-    </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A44" s="32"/>
+      <c r="P43" s="44">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A44" s="54"/>
       <c r="B44" s="12">
         <v>0.75</v>
       </c>
@@ -3498,7 +3828,7 @@
         <v>60</v>
       </c>
       <c r="K44" s="1">
-        <v>0.2</v>
+        <v>8.0000000000000004E-4</v>
       </c>
       <c r="L44" s="1">
         <v>22</v>
@@ -3509,12 +3839,15 @@
       <c r="N44" s="1">
         <v>23</v>
       </c>
-      <c r="O44" s="7">
+      <c r="O44" s="41">
         <v>1.15E-2</v>
       </c>
-    </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A45" s="32"/>
+      <c r="P44" s="44">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A45" s="54"/>
       <c r="B45" s="12">
         <v>0.79166666666666696</v>
       </c>
@@ -3546,7 +3879,7 @@
         <v>60</v>
       </c>
       <c r="K45" s="1">
-        <v>0.2</v>
+        <v>8.0000000000000004E-4</v>
       </c>
       <c r="L45" s="1">
         <v>22</v>
@@ -3557,12 +3890,15 @@
       <c r="N45" s="1">
         <v>23</v>
       </c>
-      <c r="O45" s="7">
+      <c r="O45" s="41">
         <v>1.15E-2</v>
       </c>
-    </row>
-    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A46" s="32"/>
+      <c r="P45" s="44">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="46" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A46" s="54"/>
       <c r="B46" s="12">
         <v>0.83333333333333304</v>
       </c>
@@ -3594,7 +3930,7 @@
         <v>60</v>
       </c>
       <c r="K46" s="1">
-        <v>0.2</v>
+        <v>8.0000000000000004E-4</v>
       </c>
       <c r="L46" s="1">
         <v>22</v>
@@ -3605,12 +3941,15 @@
       <c r="N46" s="1">
         <v>23</v>
       </c>
-      <c r="O46" s="7">
+      <c r="O46" s="41">
         <v>1.15E-2</v>
       </c>
-    </row>
-    <row r="47" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A47" s="32"/>
+      <c r="P46" s="44">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A47" s="54"/>
       <c r="B47" s="12">
         <v>0.875</v>
       </c>
@@ -3642,7 +3981,7 @@
         <v>60</v>
       </c>
       <c r="K47" s="1">
-        <v>0.2</v>
+        <v>8.0000000000000004E-4</v>
       </c>
       <c r="L47" s="1">
         <v>22</v>
@@ -3653,12 +3992,15 @@
       <c r="N47" s="1">
         <v>23</v>
       </c>
-      <c r="O47" s="7">
+      <c r="O47" s="41">
         <v>1.15E-2</v>
       </c>
-    </row>
-    <row r="48" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A48" s="32"/>
+      <c r="P47" s="44">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="48" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A48" s="54"/>
       <c r="B48" s="12">
         <v>0.91666666666666696</v>
       </c>
@@ -3690,7 +4032,7 @@
         <v>60</v>
       </c>
       <c r="K48" s="1">
-        <v>0.2</v>
+        <v>8.0000000000000004E-4</v>
       </c>
       <c r="L48" s="1">
         <v>22</v>
@@ -3701,12 +4043,15 @@
       <c r="N48" s="1">
         <v>23</v>
       </c>
-      <c r="O48" s="7">
+      <c r="O48" s="41">
         <v>1.15E-2</v>
       </c>
-    </row>
-    <row r="49" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A49" s="32"/>
+      <c r="P48" s="44">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="49" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A49" s="54"/>
       <c r="B49" s="12">
         <v>0.95833333333333304</v>
       </c>
@@ -3738,7 +4083,7 @@
         <v>60</v>
       </c>
       <c r="K49" s="1">
-        <v>0.2</v>
+        <v>8.0000000000000004E-4</v>
       </c>
       <c r="L49" s="1">
         <v>22</v>
@@ -3749,12 +4094,15 @@
       <c r="N49" s="1">
         <v>23</v>
       </c>
-      <c r="O49" s="7">
+      <c r="O49" s="41">
         <v>1.15E-2</v>
       </c>
-    </row>
-    <row r="50" spans="1:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="33"/>
+      <c r="P49" s="44">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="50" spans="1:16" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="55"/>
       <c r="B50" s="13">
         <v>0.999999999999999</v>
       </c>
@@ -3786,7 +4134,7 @@
         <v>60</v>
       </c>
       <c r="K50" s="9">
-        <v>0.2</v>
+        <v>8.0000000000000004E-4</v>
       </c>
       <c r="L50" s="9">
         <v>22</v>
@@ -3797,12 +4145,15 @@
       <c r="N50" s="9">
         <v>23</v>
       </c>
-      <c r="O50" s="10">
+      <c r="O50" s="42">
         <v>1.15E-2</v>
       </c>
-    </row>
-    <row r="51" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A51" s="34" t="s">
+      <c r="P50" s="45">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="51" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A51" s="56" t="s">
         <v>19</v>
       </c>
       <c r="B51" s="11">
@@ -3833,7 +4184,7 @@
         <v>60</v>
       </c>
       <c r="K51" s="2">
-        <v>0.2</v>
+        <v>8.0000000000000004E-4</v>
       </c>
       <c r="L51" s="2">
         <v>22</v>
@@ -3844,12 +4195,15 @@
       <c r="N51" s="2">
         <v>23</v>
       </c>
-      <c r="O51" s="6">
+      <c r="O51" s="40">
         <v>1.15E-2</v>
       </c>
-    </row>
-    <row r="52" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A52" s="35"/>
+      <c r="P51" s="43">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="52" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A52" s="57"/>
       <c r="B52" s="12">
         <v>8.3333333333333301E-2</v>
       </c>
@@ -3878,7 +4232,7 @@
         <v>60</v>
       </c>
       <c r="K52" s="1">
-        <v>0.2</v>
+        <v>8.0000000000000004E-4</v>
       </c>
       <c r="L52" s="1">
         <v>22</v>
@@ -3889,12 +4243,15 @@
       <c r="N52" s="1">
         <v>23</v>
       </c>
-      <c r="O52" s="7">
+      <c r="O52" s="41">
         <v>1.15E-2</v>
       </c>
-    </row>
-    <row r="53" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A53" s="35"/>
+      <c r="P52" s="44">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="53" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A53" s="57"/>
       <c r="B53" s="12">
         <v>0.125</v>
       </c>
@@ -3923,7 +4280,7 @@
         <v>60</v>
       </c>
       <c r="K53" s="1">
-        <v>0.2</v>
+        <v>8.0000000000000004E-4</v>
       </c>
       <c r="L53" s="1">
         <v>22</v>
@@ -3934,12 +4291,15 @@
       <c r="N53" s="1">
         <v>23</v>
       </c>
-      <c r="O53" s="7">
+      <c r="O53" s="41">
         <v>1.15E-2</v>
       </c>
-    </row>
-    <row r="54" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A54" s="35"/>
+      <c r="P53" s="44">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="54" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A54" s="57"/>
       <c r="B54" s="12">
         <v>0.16666666666666699</v>
       </c>
@@ -3968,7 +4328,7 @@
         <v>60</v>
       </c>
       <c r="K54" s="1">
-        <v>0.2</v>
+        <v>8.0000000000000004E-4</v>
       </c>
       <c r="L54" s="1">
         <v>22</v>
@@ -3979,12 +4339,15 @@
       <c r="N54" s="1">
         <v>23</v>
       </c>
-      <c r="O54" s="7">
+      <c r="O54" s="41">
         <v>1.15E-2</v>
       </c>
-    </row>
-    <row r="55" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A55" s="35"/>
+      <c r="P54" s="44">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="55" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A55" s="57"/>
       <c r="B55" s="12">
         <v>0.20833333333333301</v>
       </c>
@@ -4013,7 +4376,7 @@
         <v>60</v>
       </c>
       <c r="K55" s="1">
-        <v>0.2</v>
+        <v>8.0000000000000004E-4</v>
       </c>
       <c r="L55" s="1">
         <v>22</v>
@@ -4024,12 +4387,15 @@
       <c r="N55" s="1">
         <v>23</v>
       </c>
-      <c r="O55" s="7">
+      <c r="O55" s="41">
         <v>1.15E-2</v>
       </c>
-    </row>
-    <row r="56" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A56" s="35"/>
+      <c r="P55" s="44">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="56" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A56" s="57"/>
       <c r="B56" s="12">
         <v>0.25</v>
       </c>
@@ -4058,7 +4424,7 @@
         <v>60</v>
       </c>
       <c r="K56" s="1">
-        <v>0.2</v>
+        <v>8.0000000000000004E-4</v>
       </c>
       <c r="L56" s="1">
         <v>22</v>
@@ -4069,12 +4435,15 @@
       <c r="N56" s="1">
         <v>23</v>
       </c>
-      <c r="O56" s="7">
+      <c r="O56" s="41">
         <v>1.15E-2</v>
       </c>
-    </row>
-    <row r="57" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A57" s="35"/>
+      <c r="P56" s="44">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="57" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A57" s="57"/>
       <c r="B57" s="12">
         <v>0.29166666666666702</v>
       </c>
@@ -4103,7 +4472,7 @@
         <v>60</v>
       </c>
       <c r="K57" s="1">
-        <v>0.2</v>
+        <v>8.0000000000000004E-4</v>
       </c>
       <c r="L57" s="1">
         <v>22</v>
@@ -4114,12 +4483,15 @@
       <c r="N57" s="1">
         <v>23</v>
       </c>
-      <c r="O57" s="7">
+      <c r="O57" s="41">
         <v>1.15E-2</v>
       </c>
-    </row>
-    <row r="58" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A58" s="35"/>
+      <c r="P57" s="44">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="58" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A58" s="57"/>
       <c r="B58" s="12">
         <v>0.33333333333333298</v>
       </c>
@@ -4148,7 +4520,7 @@
         <v>60</v>
       </c>
       <c r="K58" s="1">
-        <v>0.2</v>
+        <v>8.0000000000000004E-4</v>
       </c>
       <c r="L58" s="1">
         <v>22</v>
@@ -4159,12 +4531,15 @@
       <c r="N58" s="1">
         <v>23</v>
       </c>
-      <c r="O58" s="7">
+      <c r="O58" s="41">
         <v>1.15E-2</v>
       </c>
-    </row>
-    <row r="59" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A59" s="35"/>
+      <c r="P58" s="44">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="59" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A59" s="57"/>
       <c r="B59" s="12">
         <v>0.375</v>
       </c>
@@ -4193,7 +4568,7 @@
         <v>60</v>
       </c>
       <c r="K59" s="1">
-        <v>0.2</v>
+        <v>8.0000000000000004E-4</v>
       </c>
       <c r="L59" s="1">
         <v>22</v>
@@ -4204,12 +4579,15 @@
       <c r="N59" s="1">
         <v>23</v>
       </c>
-      <c r="O59" s="7">
+      <c r="O59" s="41">
         <v>1.15E-2</v>
       </c>
-    </row>
-    <row r="60" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A60" s="35"/>
+      <c r="P59" s="44">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="60" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A60" s="57"/>
       <c r="B60" s="12">
         <v>0.41666666666666702</v>
       </c>
@@ -4238,7 +4616,7 @@
         <v>60</v>
       </c>
       <c r="K60" s="1">
-        <v>0.2</v>
+        <v>8.0000000000000004E-4</v>
       </c>
       <c r="L60" s="1">
         <v>22</v>
@@ -4249,12 +4627,15 @@
       <c r="N60" s="1">
         <v>23</v>
       </c>
-      <c r="O60" s="7">
+      <c r="O60" s="41">
         <v>1.15E-2</v>
       </c>
-    </row>
-    <row r="61" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A61" s="35"/>
+      <c r="P60" s="44">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="61" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A61" s="57"/>
       <c r="B61" s="12">
         <v>0.45833333333333298</v>
       </c>
@@ -4283,7 +4664,7 @@
         <v>60</v>
       </c>
       <c r="K61" s="1">
-        <v>0.2</v>
+        <v>8.0000000000000004E-4</v>
       </c>
       <c r="L61" s="1">
         <v>22</v>
@@ -4294,12 +4675,15 @@
       <c r="N61" s="1">
         <v>23</v>
       </c>
-      <c r="O61" s="7">
+      <c r="O61" s="41">
         <v>1.15E-2</v>
       </c>
-    </row>
-    <row r="62" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A62" s="35"/>
+      <c r="P61" s="44">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="62" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A62" s="57"/>
       <c r="B62" s="12">
         <v>0.5</v>
       </c>
@@ -4328,7 +4712,7 @@
         <v>60</v>
       </c>
       <c r="K62" s="1">
-        <v>0.2</v>
+        <v>8.0000000000000004E-4</v>
       </c>
       <c r="L62" s="1">
         <v>22</v>
@@ -4339,12 +4723,15 @@
       <c r="N62" s="1">
         <v>23</v>
       </c>
-      <c r="O62" s="7">
+      <c r="O62" s="41">
         <v>1.15E-2</v>
       </c>
-    </row>
-    <row r="63" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A63" s="35"/>
+      <c r="P62" s="44">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="63" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A63" s="57"/>
       <c r="B63" s="12">
         <v>0.54166666666666696</v>
       </c>
@@ -4373,7 +4760,7 @@
         <v>60</v>
       </c>
       <c r="K63" s="1">
-        <v>0.2</v>
+        <v>8.0000000000000004E-4</v>
       </c>
       <c r="L63" s="1">
         <v>22</v>
@@ -4384,12 +4771,15 @@
       <c r="N63" s="1">
         <v>23</v>
       </c>
-      <c r="O63" s="7">
+      <c r="O63" s="41">
         <v>1.15E-2</v>
       </c>
-    </row>
-    <row r="64" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A64" s="35"/>
+      <c r="P63" s="44">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="64" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A64" s="57"/>
       <c r="B64" s="12">
         <v>0.58333333333333304</v>
       </c>
@@ -4418,7 +4808,7 @@
         <v>60</v>
       </c>
       <c r="K64" s="1">
-        <v>0.2</v>
+        <v>8.0000000000000004E-4</v>
       </c>
       <c r="L64" s="1">
         <v>22</v>
@@ -4429,12 +4819,15 @@
       <c r="N64" s="1">
         <v>23</v>
       </c>
-      <c r="O64" s="7">
+      <c r="O64" s="41">
         <v>1.15E-2</v>
       </c>
-    </row>
-    <row r="65" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A65" s="35"/>
+      <c r="P64" s="44">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="65" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A65" s="57"/>
       <c r="B65" s="12">
         <v>0.625</v>
       </c>
@@ -4463,7 +4856,7 @@
         <v>60</v>
       </c>
       <c r="K65" s="1">
-        <v>0.2</v>
+        <v>8.0000000000000004E-4</v>
       </c>
       <c r="L65" s="1">
         <v>22</v>
@@ -4474,12 +4867,15 @@
       <c r="N65" s="1">
         <v>23</v>
       </c>
-      <c r="O65" s="7">
+      <c r="O65" s="41">
         <v>1.15E-2</v>
       </c>
-    </row>
-    <row r="66" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A66" s="35"/>
+      <c r="P65" s="44">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="66" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A66" s="57"/>
       <c r="B66" s="12">
         <v>0.66666666666666696</v>
       </c>
@@ -4508,7 +4904,7 @@
         <v>60</v>
       </c>
       <c r="K66" s="1">
-        <v>0.2</v>
+        <v>8.0000000000000004E-4</v>
       </c>
       <c r="L66" s="1">
         <v>22</v>
@@ -4519,12 +4915,15 @@
       <c r="N66" s="1">
         <v>23</v>
       </c>
-      <c r="O66" s="7">
+      <c r="O66" s="41">
         <v>1.15E-2</v>
       </c>
-    </row>
-    <row r="67" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A67" s="35"/>
+      <c r="P66" s="44">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="67" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A67" s="57"/>
       <c r="B67" s="12">
         <v>0.70833333333333304</v>
       </c>
@@ -4553,7 +4952,7 @@
         <v>60</v>
       </c>
       <c r="K67" s="1">
-        <v>0.2</v>
+        <v>8.0000000000000004E-4</v>
       </c>
       <c r="L67" s="1">
         <v>22</v>
@@ -4564,12 +4963,15 @@
       <c r="N67" s="1">
         <v>23</v>
       </c>
-      <c r="O67" s="7">
+      <c r="O67" s="41">
         <v>1.15E-2</v>
       </c>
-    </row>
-    <row r="68" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A68" s="35"/>
+      <c r="P67" s="44">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="68" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A68" s="57"/>
       <c r="B68" s="12">
         <v>0.75</v>
       </c>
@@ -4598,7 +5000,7 @@
         <v>60</v>
       </c>
       <c r="K68" s="1">
-        <v>0.2</v>
+        <v>8.0000000000000004E-4</v>
       </c>
       <c r="L68" s="1">
         <v>22</v>
@@ -4609,12 +5011,15 @@
       <c r="N68" s="1">
         <v>23</v>
       </c>
-      <c r="O68" s="7">
+      <c r="O68" s="41">
         <v>1.15E-2</v>
       </c>
-    </row>
-    <row r="69" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A69" s="35"/>
+      <c r="P68" s="44">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="69" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A69" s="57"/>
       <c r="B69" s="12">
         <v>0.79166666666666696</v>
       </c>
@@ -4643,7 +5048,7 @@
         <v>60</v>
       </c>
       <c r="K69" s="1">
-        <v>0.2</v>
+        <v>8.0000000000000004E-4</v>
       </c>
       <c r="L69" s="1">
         <v>22</v>
@@ -4654,12 +5059,15 @@
       <c r="N69" s="1">
         <v>23</v>
       </c>
-      <c r="O69" s="7">
+      <c r="O69" s="41">
         <v>1.15E-2</v>
       </c>
-    </row>
-    <row r="70" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A70" s="35"/>
+      <c r="P69" s="44">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="70" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A70" s="57"/>
       <c r="B70" s="12">
         <v>0.83333333333333304</v>
       </c>
@@ -4688,7 +5096,7 @@
         <v>60</v>
       </c>
       <c r="K70" s="1">
-        <v>0.2</v>
+        <v>8.0000000000000004E-4</v>
       </c>
       <c r="L70" s="1">
         <v>22</v>
@@ -4699,12 +5107,15 @@
       <c r="N70" s="1">
         <v>23</v>
       </c>
-      <c r="O70" s="7">
+      <c r="O70" s="41">
         <v>1.15E-2</v>
       </c>
-    </row>
-    <row r="71" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A71" s="35"/>
+      <c r="P70" s="44">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="71" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A71" s="57"/>
       <c r="B71" s="12">
         <v>0.875</v>
       </c>
@@ -4733,7 +5144,7 @@
         <v>60</v>
       </c>
       <c r="K71" s="1">
-        <v>0.2</v>
+        <v>8.0000000000000004E-4</v>
       </c>
       <c r="L71" s="1">
         <v>22</v>
@@ -4744,12 +5155,15 @@
       <c r="N71" s="1">
         <v>23</v>
       </c>
-      <c r="O71" s="7">
+      <c r="O71" s="41">
         <v>1.15E-2</v>
       </c>
-    </row>
-    <row r="72" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A72" s="35"/>
+      <c r="P71" s="44">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="72" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A72" s="57"/>
       <c r="B72" s="12">
         <v>0.91666666666666696</v>
       </c>
@@ -4778,7 +5192,7 @@
         <v>60</v>
       </c>
       <c r="K72" s="1">
-        <v>0.2</v>
+        <v>8.0000000000000004E-4</v>
       </c>
       <c r="L72" s="1">
         <v>22</v>
@@ -4789,12 +5203,15 @@
       <c r="N72" s="1">
         <v>23</v>
       </c>
-      <c r="O72" s="7">
+      <c r="O72" s="41">
         <v>1.15E-2</v>
       </c>
-    </row>
-    <row r="73" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A73" s="35"/>
+      <c r="P72" s="44">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="73" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A73" s="57"/>
       <c r="B73" s="12">
         <v>0.95833333333333304</v>
       </c>
@@ -4823,7 +5240,7 @@
         <v>60</v>
       </c>
       <c r="K73" s="1">
-        <v>0.2</v>
+        <v>8.0000000000000004E-4</v>
       </c>
       <c r="L73" s="1">
         <v>22</v>
@@ -4834,12 +5251,15 @@
       <c r="N73" s="1">
         <v>23</v>
       </c>
-      <c r="O73" s="7">
+      <c r="O73" s="41">
         <v>1.15E-2</v>
       </c>
-    </row>
-    <row r="74" spans="1:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A74" s="36"/>
+      <c r="P73" s="44">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="74" spans="1:16" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A74" s="58"/>
       <c r="B74" s="13">
         <v>0.999999999999999</v>
       </c>
@@ -4868,7 +5288,7 @@
         <v>60</v>
       </c>
       <c r="K74" s="9">
-        <v>0.2</v>
+        <v>8.0000000000000004E-4</v>
       </c>
       <c r="L74" s="9">
         <v>22</v>
@@ -4879,8 +5299,11 @@
       <c r="N74" s="9">
         <v>23</v>
       </c>
-      <c r="O74" s="10">
+      <c r="O74" s="42">
         <v>1.15E-2</v>
+      </c>
+      <c r="P74" s="45">
+        <v>0.01</v>
       </c>
     </row>
   </sheetData>
@@ -4897,8 +5320,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89776361-7464-4832-9F9A-04759F7BF64E}">
   <dimension ref="A1:AS74"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="M9" sqref="M9"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="P3" sqref="P3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -4920,75 +5343,77 @@
       <c r="B1" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="C1" s="22" t="s">
-        <v>26</v>
-      </c>
-      <c r="D1" s="21" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" s="23" t="s">
+      <c r="C1" s="29" t="s">
+        <v>26</v>
+      </c>
+      <c r="D1" s="30" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="23" t="s">
+      <c r="F1" s="31" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="22" t="s">
+      <c r="G1" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="23" t="s">
+      <c r="H1" s="33" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="23" t="s">
+      <c r="I1" s="33" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="21" t="s">
+      <c r="J1" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="21" t="s">
+      <c r="K1" s="35" t="s">
         <v>4</v>
       </c>
-      <c r="L1" s="21" t="s">
+      <c r="L1" s="35" t="s">
         <v>28</v>
       </c>
-      <c r="M1" s="21" t="s">
+      <c r="M1" s="35" t="s">
         <v>29</v>
       </c>
-      <c r="N1" s="21" t="s">
+      <c r="N1" s="35" t="s">
         <v>30</v>
       </c>
-      <c r="O1" s="21" t="s">
+      <c r="O1" s="39" t="s">
         <v>31</v>
       </c>
-      <c r="P1" s="24"/>
-      <c r="Q1" s="24"/>
-      <c r="R1" s="24"/>
-      <c r="S1" s="24"/>
-      <c r="T1" s="24"/>
-      <c r="U1" s="24"/>
-      <c r="V1" s="24"/>
-      <c r="W1" s="24"/>
-      <c r="X1" s="24"/>
-      <c r="Y1" s="24"/>
-      <c r="Z1" s="24"/>
-      <c r="AA1" s="24"/>
-      <c r="AB1" s="24"/>
-      <c r="AC1" s="24"/>
-      <c r="AD1" s="24"/>
-      <c r="AE1" s="24"/>
-      <c r="AF1" s="24"/>
-      <c r="AG1" s="24"/>
-      <c r="AH1" s="25"/>
-      <c r="AI1" s="25"/>
-      <c r="AJ1" s="25"/>
-      <c r="AK1" s="25"/>
-      <c r="AL1" s="25"/>
-      <c r="AM1" s="25"/>
-      <c r="AN1" s="25"/>
-      <c r="AO1" s="25"/>
-      <c r="AP1" s="25"/>
-      <c r="AQ1" s="25"/>
-      <c r="AR1" s="25"/>
-      <c r="AS1" s="25"/>
+      <c r="P1" s="38" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q1" s="22"/>
+      <c r="R1" s="22"/>
+      <c r="S1" s="22"/>
+      <c r="T1" s="22"/>
+      <c r="U1" s="22"/>
+      <c r="V1" s="22"/>
+      <c r="W1" s="22"/>
+      <c r="X1" s="22"/>
+      <c r="Y1" s="22"/>
+      <c r="Z1" s="22"/>
+      <c r="AA1" s="22"/>
+      <c r="AB1" s="22"/>
+      <c r="AC1" s="22"/>
+      <c r="AD1" s="22"/>
+      <c r="AE1" s="22"/>
+      <c r="AF1" s="22"/>
+      <c r="AG1" s="22"/>
+      <c r="AH1" s="23"/>
+      <c r="AI1" s="23"/>
+      <c r="AJ1" s="23"/>
+      <c r="AK1" s="23"/>
+      <c r="AL1" s="23"/>
+      <c r="AM1" s="23"/>
+      <c r="AN1" s="23"/>
+      <c r="AO1" s="23"/>
+      <c r="AP1" s="23"/>
+      <c r="AQ1" s="23"/>
+      <c r="AR1" s="23"/>
+      <c r="AS1" s="23"/>
     </row>
     <row r="2" spans="1:45" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="5" t="s">
@@ -5033,7 +5458,9 @@
       <c r="O2" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="P2" s="16"/>
+      <c r="P2" s="37" t="s">
+        <v>38</v>
+      </c>
       <c r="Q2" s="16"/>
       <c r="R2" s="16"/>
       <c r="S2" s="16"/>
@@ -5065,7 +5492,7 @@
       <c r="AS2" s="15"/>
     </row>
     <row r="3" spans="1:45" x14ac:dyDescent="0.25">
-      <c r="A3" s="28" t="s">
+      <c r="A3" s="50" t="s">
         <v>0</v>
       </c>
       <c r="B3" s="11">
@@ -5096,7 +5523,7 @@
         <v>60</v>
       </c>
       <c r="K3" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L3" s="2">
         <v>22</v>
@@ -5110,7 +5537,9 @@
       <c r="O3" s="6">
         <v>1.0500000000000001E-2</v>
       </c>
-      <c r="P3" s="15"/>
+      <c r="P3" s="43">
+        <v>0</v>
+      </c>
       <c r="Q3" s="15"/>
       <c r="R3" s="15"/>
       <c r="S3" s="15"/>
@@ -5142,7 +5571,7 @@
       <c r="AS3" s="15"/>
     </row>
     <row r="4" spans="1:45" x14ac:dyDescent="0.25">
-      <c r="A4" s="29"/>
+      <c r="A4" s="51"/>
       <c r="B4" s="12">
         <v>8.3333333333333301E-2</v>
       </c>
@@ -5171,7 +5600,7 @@
         <v>60</v>
       </c>
       <c r="K4" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L4" s="1">
         <v>22</v>
@@ -5185,7 +5614,9 @@
       <c r="O4" s="7">
         <v>1.0500000000000001E-2</v>
       </c>
-      <c r="P4" s="15"/>
+      <c r="P4" s="44">
+        <v>0</v>
+      </c>
       <c r="Q4" s="15"/>
       <c r="R4" s="15"/>
       <c r="S4" s="15"/>
@@ -5217,7 +5648,7 @@
       <c r="AS4" s="15"/>
     </row>
     <row r="5" spans="1:45" x14ac:dyDescent="0.25">
-      <c r="A5" s="29"/>
+      <c r="A5" s="51"/>
       <c r="B5" s="12">
         <v>0.125</v>
       </c>
@@ -5246,7 +5677,7 @@
         <v>60</v>
       </c>
       <c r="K5" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L5" s="1">
         <v>22</v>
@@ -5260,7 +5691,9 @@
       <c r="O5" s="7">
         <v>1.0500000000000001E-2</v>
       </c>
-      <c r="P5" s="15"/>
+      <c r="P5" s="44">
+        <v>0</v>
+      </c>
       <c r="Q5" s="15"/>
       <c r="R5" s="15"/>
       <c r="S5" s="15"/>
@@ -5292,7 +5725,7 @@
       <c r="AS5" s="15"/>
     </row>
     <row r="6" spans="1:45" x14ac:dyDescent="0.25">
-      <c r="A6" s="29"/>
+      <c r="A6" s="51"/>
       <c r="B6" s="12">
         <v>0.16666666666666699</v>
       </c>
@@ -5321,7 +5754,7 @@
         <v>60</v>
       </c>
       <c r="K6" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L6" s="1">
         <v>22</v>
@@ -5335,7 +5768,9 @@
       <c r="O6" s="7">
         <v>1.0500000000000001E-2</v>
       </c>
-      <c r="P6" s="15"/>
+      <c r="P6" s="44">
+        <v>0</v>
+      </c>
       <c r="Q6" s="15"/>
       <c r="R6" s="15"/>
       <c r="S6" s="15"/>
@@ -5367,7 +5802,7 @@
       <c r="AS6" s="15"/>
     </row>
     <row r="7" spans="1:45" x14ac:dyDescent="0.25">
-      <c r="A7" s="29"/>
+      <c r="A7" s="51"/>
       <c r="B7" s="12">
         <v>0.20833333333333301</v>
       </c>
@@ -5396,7 +5831,7 @@
         <v>60</v>
       </c>
       <c r="K7" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L7" s="1">
         <v>22</v>
@@ -5410,7 +5845,9 @@
       <c r="O7" s="7">
         <v>1.0500000000000001E-2</v>
       </c>
-      <c r="P7" s="15"/>
+      <c r="P7" s="44">
+        <v>0</v>
+      </c>
       <c r="Q7" s="15"/>
       <c r="R7" s="15"/>
       <c r="S7" s="15"/>
@@ -5442,7 +5879,7 @@
       <c r="AS7" s="15"/>
     </row>
     <row r="8" spans="1:45" x14ac:dyDescent="0.25">
-      <c r="A8" s="29"/>
+      <c r="A8" s="51"/>
       <c r="B8" s="12">
         <v>0.25</v>
       </c>
@@ -5471,7 +5908,7 @@
         <v>60</v>
       </c>
       <c r="K8" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L8" s="1">
         <v>22</v>
@@ -5485,7 +5922,9 @@
       <c r="O8" s="7">
         <v>1.0500000000000001E-2</v>
       </c>
-      <c r="P8" s="15"/>
+      <c r="P8" s="44">
+        <v>0</v>
+      </c>
       <c r="Q8" s="15"/>
       <c r="R8" s="15"/>
       <c r="S8" s="15"/>
@@ -5517,7 +5956,7 @@
       <c r="AS8" s="15"/>
     </row>
     <row r="9" spans="1:45" x14ac:dyDescent="0.25">
-      <c r="A9" s="29"/>
+      <c r="A9" s="51"/>
       <c r="B9" s="12">
         <v>0.29166666666666702</v>
       </c>
@@ -5546,7 +5985,7 @@
         <v>60</v>
       </c>
       <c r="K9" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L9" s="1">
         <v>22</v>
@@ -5560,7 +5999,9 @@
       <c r="O9" s="7">
         <v>1.0500000000000001E-2</v>
       </c>
-      <c r="P9" s="15"/>
+      <c r="P9" s="44">
+        <v>0</v>
+      </c>
       <c r="Q9" s="15"/>
       <c r="R9" s="15"/>
       <c r="S9" s="15"/>
@@ -5592,7 +6033,7 @@
       <c r="AS9" s="15"/>
     </row>
     <row r="10" spans="1:45" x14ac:dyDescent="0.25">
-      <c r="A10" s="29"/>
+      <c r="A10" s="51"/>
       <c r="B10" s="12">
         <v>0.33333333333333298</v>
       </c>
@@ -5621,7 +6062,7 @@
         <v>60</v>
       </c>
       <c r="K10" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L10" s="1">
         <v>22</v>
@@ -5635,7 +6076,9 @@
       <c r="O10" s="7">
         <v>1.0500000000000001E-2</v>
       </c>
-      <c r="P10" s="15"/>
+      <c r="P10" s="44">
+        <v>0</v>
+      </c>
       <c r="Q10" s="15"/>
       <c r="R10" s="15"/>
       <c r="S10" s="15"/>
@@ -5667,7 +6110,7 @@
       <c r="AS10" s="15"/>
     </row>
     <row r="11" spans="1:45" x14ac:dyDescent="0.25">
-      <c r="A11" s="29"/>
+      <c r="A11" s="51"/>
       <c r="B11" s="12">
         <v>0.375</v>
       </c>
@@ -5696,7 +6139,7 @@
         <v>60</v>
       </c>
       <c r="K11" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L11" s="1">
         <v>22</v>
@@ -5710,9 +6153,12 @@
       <c r="O11" s="7">
         <v>1.0500000000000001E-2</v>
       </c>
+      <c r="P11" s="44">
+        <v>0</v>
+      </c>
     </row>
     <row r="12" spans="1:45" x14ac:dyDescent="0.25">
-      <c r="A12" s="29"/>
+      <c r="A12" s="51"/>
       <c r="B12" s="12">
         <v>0.41666666666666702</v>
       </c>
@@ -5741,7 +6187,7 @@
         <v>60</v>
       </c>
       <c r="K12" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L12" s="1">
         <v>22</v>
@@ -5755,9 +6201,12 @@
       <c r="O12" s="7">
         <v>1.0500000000000001E-2</v>
       </c>
+      <c r="P12" s="44">
+        <v>0</v>
+      </c>
     </row>
     <row r="13" spans="1:45" x14ac:dyDescent="0.25">
-      <c r="A13" s="29"/>
+      <c r="A13" s="51"/>
       <c r="B13" s="12">
         <v>0.45833333333333298</v>
       </c>
@@ -5786,7 +6235,7 @@
         <v>60</v>
       </c>
       <c r="K13" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L13" s="1">
         <v>22</v>
@@ -5800,9 +6249,12 @@
       <c r="O13" s="7">
         <v>1.0500000000000001E-2</v>
       </c>
+      <c r="P13" s="44">
+        <v>0</v>
+      </c>
     </row>
     <row r="14" spans="1:45" x14ac:dyDescent="0.25">
-      <c r="A14" s="29"/>
+      <c r="A14" s="51"/>
       <c r="B14" s="12">
         <v>0.5</v>
       </c>
@@ -5831,7 +6283,7 @@
         <v>60</v>
       </c>
       <c r="K14" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L14" s="1">
         <v>22</v>
@@ -5845,9 +6297,12 @@
       <c r="O14" s="7">
         <v>1.0500000000000001E-2</v>
       </c>
+      <c r="P14" s="44">
+        <v>0</v>
+      </c>
     </row>
     <row r="15" spans="1:45" x14ac:dyDescent="0.25">
-      <c r="A15" s="29"/>
+      <c r="A15" s="51"/>
       <c r="B15" s="12">
         <v>0.54166666666666696</v>
       </c>
@@ -5876,7 +6331,7 @@
         <v>60</v>
       </c>
       <c r="K15" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L15" s="1">
         <v>22</v>
@@ -5890,9 +6345,12 @@
       <c r="O15" s="7">
         <v>1.0500000000000001E-2</v>
       </c>
+      <c r="P15" s="44">
+        <v>0</v>
+      </c>
     </row>
     <row r="16" spans="1:45" x14ac:dyDescent="0.25">
-      <c r="A16" s="29"/>
+      <c r="A16" s="51"/>
       <c r="B16" s="12">
         <v>0.58333333333333304</v>
       </c>
@@ -5921,7 +6379,7 @@
         <v>60</v>
       </c>
       <c r="K16" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L16" s="1">
         <v>22</v>
@@ -5935,9 +6393,12 @@
       <c r="O16" s="7">
         <v>1.0500000000000001E-2</v>
       </c>
-    </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A17" s="29"/>
+      <c r="P16" s="44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A17" s="51"/>
       <c r="B17" s="12">
         <v>0.625</v>
       </c>
@@ -5966,7 +6427,7 @@
         <v>60</v>
       </c>
       <c r="K17" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L17" s="1">
         <v>22</v>
@@ -5980,9 +6441,12 @@
       <c r="O17" s="7">
         <v>1.0500000000000001E-2</v>
       </c>
-    </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A18" s="29"/>
+      <c r="P17" s="44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A18" s="51"/>
       <c r="B18" s="12">
         <v>0.66666666666666696</v>
       </c>
@@ -6011,7 +6475,7 @@
         <v>60</v>
       </c>
       <c r="K18" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L18" s="1">
         <v>22</v>
@@ -6025,9 +6489,12 @@
       <c r="O18" s="7">
         <v>1.0500000000000001E-2</v>
       </c>
-    </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A19" s="29"/>
+      <c r="P18" s="44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A19" s="51"/>
       <c r="B19" s="12">
         <v>0.70833333333333304</v>
       </c>
@@ -6056,7 +6523,7 @@
         <v>60</v>
       </c>
       <c r="K19" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L19" s="1">
         <v>22</v>
@@ -6070,9 +6537,12 @@
       <c r="O19" s="7">
         <v>1.0500000000000001E-2</v>
       </c>
-    </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A20" s="29"/>
+      <c r="P19" s="44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A20" s="51"/>
       <c r="B20" s="12">
         <v>0.75</v>
       </c>
@@ -6101,7 +6571,7 @@
         <v>60</v>
       </c>
       <c r="K20" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L20" s="1">
         <v>22</v>
@@ -6115,9 +6585,12 @@
       <c r="O20" s="7">
         <v>1.0500000000000001E-2</v>
       </c>
-    </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A21" s="29"/>
+      <c r="P20" s="44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A21" s="51"/>
       <c r="B21" s="12">
         <v>0.79166666666666696</v>
       </c>
@@ -6146,7 +6619,7 @@
         <v>60</v>
       </c>
       <c r="K21" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L21" s="1">
         <v>22</v>
@@ -6160,9 +6633,12 @@
       <c r="O21" s="7">
         <v>1.0500000000000001E-2</v>
       </c>
-    </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A22" s="29"/>
+      <c r="P21" s="44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A22" s="51"/>
       <c r="B22" s="12">
         <v>0.83333333333333304</v>
       </c>
@@ -6191,7 +6667,7 @@
         <v>60</v>
       </c>
       <c r="K22" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L22" s="1">
         <v>22</v>
@@ -6205,9 +6681,12 @@
       <c r="O22" s="7">
         <v>1.0500000000000001E-2</v>
       </c>
-    </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A23" s="29"/>
+      <c r="P22" s="44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A23" s="51"/>
       <c r="B23" s="12">
         <v>0.875</v>
       </c>
@@ -6236,7 +6715,7 @@
         <v>60</v>
       </c>
       <c r="K23" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L23" s="1">
         <v>22</v>
@@ -6250,9 +6729,12 @@
       <c r="O23" s="7">
         <v>1.0500000000000001E-2</v>
       </c>
-    </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A24" s="29"/>
+      <c r="P23" s="44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A24" s="51"/>
       <c r="B24" s="12">
         <v>0.91666666666666696</v>
       </c>
@@ -6281,7 +6763,7 @@
         <v>60</v>
       </c>
       <c r="K24" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L24" s="1">
         <v>22</v>
@@ -6295,9 +6777,12 @@
       <c r="O24" s="7">
         <v>1.0500000000000001E-2</v>
       </c>
-    </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A25" s="29"/>
+      <c r="P24" s="44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A25" s="51"/>
       <c r="B25" s="12">
         <v>0.95833333333333304</v>
       </c>
@@ -6326,7 +6811,7 @@
         <v>60</v>
       </c>
       <c r="K25" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L25" s="1">
         <v>22</v>
@@ -6340,9 +6825,12 @@
       <c r="O25" s="7">
         <v>1.0500000000000001E-2</v>
       </c>
-    </row>
-    <row r="26" spans="1:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="30"/>
+      <c r="P25" s="44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="52"/>
       <c r="B26" s="13">
         <v>0.999999999999999</v>
       </c>
@@ -6371,7 +6859,7 @@
         <v>60</v>
       </c>
       <c r="K26" s="8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L26" s="9">
         <v>22</v>
@@ -6385,9 +6873,12 @@
       <c r="O26" s="10">
         <v>1.0500000000000001E-2</v>
       </c>
-    </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A27" s="31" t="s">
+      <c r="P26" s="45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A27" s="53" t="s">
         <v>18</v>
       </c>
       <c r="B27" s="11">
@@ -6418,7 +6909,7 @@
         <v>60</v>
       </c>
       <c r="K27" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L27" s="2">
         <v>22</v>
@@ -6432,9 +6923,12 @@
       <c r="O27" s="6">
         <v>1.0500000000000001E-2</v>
       </c>
-    </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A28" s="32"/>
+      <c r="P27" s="43">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A28" s="54"/>
       <c r="B28" s="12">
         <v>8.3333333333333301E-2</v>
       </c>
@@ -6463,7 +6957,7 @@
         <v>60</v>
       </c>
       <c r="K28" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L28" s="1">
         <v>22</v>
@@ -6477,9 +6971,12 @@
       <c r="O28" s="7">
         <v>1.0500000000000001E-2</v>
       </c>
-    </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A29" s="32"/>
+      <c r="P28" s="44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A29" s="54"/>
       <c r="B29" s="12">
         <v>0.125</v>
       </c>
@@ -6508,7 +7005,7 @@
         <v>60</v>
       </c>
       <c r="K29" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L29" s="1">
         <v>22</v>
@@ -6522,9 +7019,12 @@
       <c r="O29" s="7">
         <v>1.0500000000000001E-2</v>
       </c>
-    </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A30" s="32"/>
+      <c r="P29" s="44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A30" s="54"/>
       <c r="B30" s="12">
         <v>0.16666666666666699</v>
       </c>
@@ -6553,7 +7053,7 @@
         <v>60</v>
       </c>
       <c r="K30" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L30" s="1">
         <v>22</v>
@@ -6567,9 +7067,12 @@
       <c r="O30" s="7">
         <v>1.0500000000000001E-2</v>
       </c>
-    </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A31" s="32"/>
+      <c r="P30" s="44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A31" s="54"/>
       <c r="B31" s="12">
         <v>0.20833333333333301</v>
       </c>
@@ -6598,7 +7101,7 @@
         <v>60</v>
       </c>
       <c r="K31" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L31" s="1">
         <v>22</v>
@@ -6612,9 +7115,12 @@
       <c r="O31" s="7">
         <v>1.0500000000000001E-2</v>
       </c>
-    </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A32" s="32"/>
+      <c r="P31" s="44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A32" s="54"/>
       <c r="B32" s="12">
         <v>0.25</v>
       </c>
@@ -6643,7 +7149,7 @@
         <v>60</v>
       </c>
       <c r="K32" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L32" s="1">
         <v>22</v>
@@ -6657,9 +7163,12 @@
       <c r="O32" s="7">
         <v>1.0500000000000001E-2</v>
       </c>
-    </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A33" s="32"/>
+      <c r="P32" s="44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A33" s="54"/>
       <c r="B33" s="12">
         <v>0.29166666666666702</v>
       </c>
@@ -6688,7 +7197,7 @@
         <v>60</v>
       </c>
       <c r="K33" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L33" s="1">
         <v>22</v>
@@ -6702,9 +7211,12 @@
       <c r="O33" s="7">
         <v>1.0500000000000001E-2</v>
       </c>
-    </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A34" s="32"/>
+      <c r="P33" s="44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A34" s="54"/>
       <c r="B34" s="12">
         <v>0.33333333333333298</v>
       </c>
@@ -6733,7 +7245,7 @@
         <v>60</v>
       </c>
       <c r="K34" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L34" s="1">
         <v>22</v>
@@ -6747,9 +7259,12 @@
       <c r="O34" s="7">
         <v>1.0500000000000001E-2</v>
       </c>
-    </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A35" s="32"/>
+      <c r="P34" s="44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A35" s="54"/>
       <c r="B35" s="12">
         <v>0.375</v>
       </c>
@@ -6778,7 +7293,7 @@
         <v>60</v>
       </c>
       <c r="K35" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L35" s="1">
         <v>22</v>
@@ -6792,9 +7307,12 @@
       <c r="O35" s="7">
         <v>1.0500000000000001E-2</v>
       </c>
-    </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A36" s="32"/>
+      <c r="P35" s="44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A36" s="54"/>
       <c r="B36" s="12">
         <v>0.41666666666666702</v>
       </c>
@@ -6823,7 +7341,7 @@
         <v>60</v>
       </c>
       <c r="K36" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L36" s="1">
         <v>22</v>
@@ -6837,9 +7355,12 @@
       <c r="O36" s="7">
         <v>1.0500000000000001E-2</v>
       </c>
-    </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A37" s="32"/>
+      <c r="P36" s="44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A37" s="54"/>
       <c r="B37" s="12">
         <v>0.45833333333333298</v>
       </c>
@@ -6868,7 +7389,7 @@
         <v>60</v>
       </c>
       <c r="K37" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L37" s="1">
         <v>22</v>
@@ -6882,9 +7403,12 @@
       <c r="O37" s="7">
         <v>1.0500000000000001E-2</v>
       </c>
-    </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A38" s="32"/>
+      <c r="P37" s="44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A38" s="54"/>
       <c r="B38" s="12">
         <v>0.5</v>
       </c>
@@ -6913,7 +7437,7 @@
         <v>60</v>
       </c>
       <c r="K38" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L38" s="1">
         <v>22</v>
@@ -6927,9 +7451,12 @@
       <c r="O38" s="7">
         <v>1.0500000000000001E-2</v>
       </c>
-    </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A39" s="32"/>
+      <c r="P38" s="44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A39" s="54"/>
       <c r="B39" s="12">
         <v>0.54166666666666696</v>
       </c>
@@ -6958,7 +7485,7 @@
         <v>60</v>
       </c>
       <c r="K39" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L39" s="1">
         <v>22</v>
@@ -6972,9 +7499,12 @@
       <c r="O39" s="7">
         <v>1.0500000000000001E-2</v>
       </c>
-    </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A40" s="32"/>
+      <c r="P39" s="44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A40" s="54"/>
       <c r="B40" s="12">
         <v>0.58333333333333304</v>
       </c>
@@ -7003,7 +7533,7 @@
         <v>60</v>
       </c>
       <c r="K40" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L40" s="1">
         <v>22</v>
@@ -7017,9 +7547,12 @@
       <c r="O40" s="7">
         <v>1.0500000000000001E-2</v>
       </c>
-    </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A41" s="32"/>
+      <c r="P40" s="44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A41" s="54"/>
       <c r="B41" s="12">
         <v>0.625</v>
       </c>
@@ -7048,7 +7581,7 @@
         <v>60</v>
       </c>
       <c r="K41" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L41" s="1">
         <v>22</v>
@@ -7062,9 +7595,12 @@
       <c r="O41" s="7">
         <v>1.0500000000000001E-2</v>
       </c>
-    </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A42" s="32"/>
+      <c r="P41" s="44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A42" s="54"/>
       <c r="B42" s="12">
         <v>0.66666666666666696</v>
       </c>
@@ -7093,7 +7629,7 @@
         <v>60</v>
       </c>
       <c r="K42" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L42" s="1">
         <v>22</v>
@@ -7107,9 +7643,12 @@
       <c r="O42" s="7">
         <v>1.0500000000000001E-2</v>
       </c>
-    </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A43" s="32"/>
+      <c r="P42" s="44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A43" s="54"/>
       <c r="B43" s="12">
         <v>0.70833333333333304</v>
       </c>
@@ -7138,7 +7677,7 @@
         <v>60</v>
       </c>
       <c r="K43" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L43" s="1">
         <v>22</v>
@@ -7152,9 +7691,12 @@
       <c r="O43" s="7">
         <v>1.0500000000000001E-2</v>
       </c>
-    </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A44" s="32"/>
+      <c r="P43" s="44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A44" s="54"/>
       <c r="B44" s="12">
         <v>0.75</v>
       </c>
@@ -7183,7 +7725,7 @@
         <v>60</v>
       </c>
       <c r="K44" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L44" s="1">
         <v>22</v>
@@ -7197,9 +7739,12 @@
       <c r="O44" s="7">
         <v>1.0500000000000001E-2</v>
       </c>
-    </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A45" s="32"/>
+      <c r="P44" s="44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A45" s="54"/>
       <c r="B45" s="12">
         <v>0.79166666666666696</v>
       </c>
@@ -7228,7 +7773,7 @@
         <v>60</v>
       </c>
       <c r="K45" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L45" s="1">
         <v>22</v>
@@ -7242,9 +7787,12 @@
       <c r="O45" s="7">
         <v>1.0500000000000001E-2</v>
       </c>
-    </row>
-    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A46" s="32"/>
+      <c r="P45" s="44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A46" s="54"/>
       <c r="B46" s="12">
         <v>0.83333333333333304</v>
       </c>
@@ -7273,7 +7821,7 @@
         <v>60</v>
       </c>
       <c r="K46" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L46" s="1">
         <v>22</v>
@@ -7287,9 +7835,12 @@
       <c r="O46" s="7">
         <v>1.0500000000000001E-2</v>
       </c>
-    </row>
-    <row r="47" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A47" s="32"/>
+      <c r="P46" s="44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A47" s="54"/>
       <c r="B47" s="12">
         <v>0.875</v>
       </c>
@@ -7318,7 +7869,7 @@
         <v>60</v>
       </c>
       <c r="K47" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L47" s="1">
         <v>22</v>
@@ -7332,9 +7883,12 @@
       <c r="O47" s="7">
         <v>1.0500000000000001E-2</v>
       </c>
-    </row>
-    <row r="48" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A48" s="32"/>
+      <c r="P47" s="44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A48" s="54"/>
       <c r="B48" s="12">
         <v>0.91666666666666696</v>
       </c>
@@ -7363,7 +7917,7 @@
         <v>60</v>
       </c>
       <c r="K48" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L48" s="1">
         <v>22</v>
@@ -7377,9 +7931,12 @@
       <c r="O48" s="7">
         <v>1.0500000000000001E-2</v>
       </c>
-    </row>
-    <row r="49" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A49" s="32"/>
+      <c r="P48" s="44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A49" s="54"/>
       <c r="B49" s="12">
         <v>0.95833333333333304</v>
       </c>
@@ -7408,7 +7965,7 @@
         <v>60</v>
       </c>
       <c r="K49" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L49" s="1">
         <v>22</v>
@@ -7422,9 +7979,12 @@
       <c r="O49" s="7">
         <v>1.0500000000000001E-2</v>
       </c>
-    </row>
-    <row r="50" spans="1:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="33"/>
+      <c r="P49" s="44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:16" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="55"/>
       <c r="B50" s="13">
         <v>0.999999999999999</v>
       </c>
@@ -7453,7 +8013,7 @@
         <v>60</v>
       </c>
       <c r="K50" s="8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L50" s="9">
         <v>22</v>
@@ -7467,9 +8027,12 @@
       <c r="O50" s="10">
         <v>1.0500000000000001E-2</v>
       </c>
-    </row>
-    <row r="51" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A51" s="34" t="s">
+      <c r="P50" s="45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A51" s="56" t="s">
         <v>19</v>
       </c>
       <c r="B51" s="11">
@@ -7500,7 +8063,7 @@
         <v>60</v>
       </c>
       <c r="K51" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L51" s="2">
         <v>22</v>
@@ -7514,9 +8077,12 @@
       <c r="O51" s="6">
         <v>1.0500000000000001E-2</v>
       </c>
-    </row>
-    <row r="52" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A52" s="35"/>
+      <c r="P51" s="43">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A52" s="57"/>
       <c r="B52" s="12">
         <v>8.3333333333333301E-2</v>
       </c>
@@ -7545,7 +8111,7 @@
         <v>60</v>
       </c>
       <c r="K52" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L52" s="1">
         <v>22</v>
@@ -7559,9 +8125,12 @@
       <c r="O52" s="7">
         <v>1.0500000000000001E-2</v>
       </c>
-    </row>
-    <row r="53" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A53" s="35"/>
+      <c r="P52" s="44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A53" s="57"/>
       <c r="B53" s="12">
         <v>0.125</v>
       </c>
@@ -7590,7 +8159,7 @@
         <v>60</v>
       </c>
       <c r="K53" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L53" s="1">
         <v>22</v>
@@ -7604,9 +8173,12 @@
       <c r="O53" s="7">
         <v>1.0500000000000001E-2</v>
       </c>
-    </row>
-    <row r="54" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A54" s="35"/>
+      <c r="P53" s="44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A54" s="57"/>
       <c r="B54" s="12">
         <v>0.16666666666666699</v>
       </c>
@@ -7635,7 +8207,7 @@
         <v>60</v>
       </c>
       <c r="K54" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L54" s="1">
         <v>22</v>
@@ -7649,9 +8221,12 @@
       <c r="O54" s="7">
         <v>1.0500000000000001E-2</v>
       </c>
-    </row>
-    <row r="55" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A55" s="35"/>
+      <c r="P54" s="44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A55" s="57"/>
       <c r="B55" s="12">
         <v>0.20833333333333301</v>
       </c>
@@ -7680,7 +8255,7 @@
         <v>60</v>
       </c>
       <c r="K55" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L55" s="1">
         <v>22</v>
@@ -7694,9 +8269,12 @@
       <c r="O55" s="7">
         <v>1.0500000000000001E-2</v>
       </c>
-    </row>
-    <row r="56" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A56" s="35"/>
+      <c r="P55" s="44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A56" s="57"/>
       <c r="B56" s="12">
         <v>0.25</v>
       </c>
@@ -7725,7 +8303,7 @@
         <v>60</v>
       </c>
       <c r="K56" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L56" s="1">
         <v>22</v>
@@ -7739,9 +8317,12 @@
       <c r="O56" s="7">
         <v>1.0500000000000001E-2</v>
       </c>
-    </row>
-    <row r="57" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A57" s="35"/>
+      <c r="P56" s="44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A57" s="57"/>
       <c r="B57" s="12">
         <v>0.29166666666666702</v>
       </c>
@@ -7770,7 +8351,7 @@
         <v>60</v>
       </c>
       <c r="K57" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L57" s="1">
         <v>22</v>
@@ -7784,9 +8365,12 @@
       <c r="O57" s="7">
         <v>1.0500000000000001E-2</v>
       </c>
-    </row>
-    <row r="58" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A58" s="35"/>
+      <c r="P57" s="44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A58" s="57"/>
       <c r="B58" s="12">
         <v>0.33333333333333298</v>
       </c>
@@ -7815,7 +8399,7 @@
         <v>60</v>
       </c>
       <c r="K58" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L58" s="1">
         <v>22</v>
@@ -7829,9 +8413,12 @@
       <c r="O58" s="7">
         <v>1.0500000000000001E-2</v>
       </c>
-    </row>
-    <row r="59" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A59" s="35"/>
+      <c r="P58" s="44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A59" s="57"/>
       <c r="B59" s="12">
         <v>0.375</v>
       </c>
@@ -7860,7 +8447,7 @@
         <v>60</v>
       </c>
       <c r="K59" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L59" s="1">
         <v>22</v>
@@ -7874,9 +8461,12 @@
       <c r="O59" s="7">
         <v>1.0500000000000001E-2</v>
       </c>
-    </row>
-    <row r="60" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A60" s="35"/>
+      <c r="P59" s="44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A60" s="57"/>
       <c r="B60" s="12">
         <v>0.41666666666666702</v>
       </c>
@@ -7905,7 +8495,7 @@
         <v>60</v>
       </c>
       <c r="K60" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L60" s="1">
         <v>22</v>
@@ -7919,9 +8509,12 @@
       <c r="O60" s="7">
         <v>1.0500000000000001E-2</v>
       </c>
-    </row>
-    <row r="61" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A61" s="35"/>
+      <c r="P60" s="44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A61" s="57"/>
       <c r="B61" s="12">
         <v>0.45833333333333298</v>
       </c>
@@ -7950,7 +8543,7 @@
         <v>60</v>
       </c>
       <c r="K61" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L61" s="1">
         <v>22</v>
@@ -7964,9 +8557,12 @@
       <c r="O61" s="7">
         <v>1.0500000000000001E-2</v>
       </c>
-    </row>
-    <row r="62" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A62" s="35"/>
+      <c r="P61" s="44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A62" s="57"/>
       <c r="B62" s="12">
         <v>0.5</v>
       </c>
@@ -7995,7 +8591,7 @@
         <v>60</v>
       </c>
       <c r="K62" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L62" s="1">
         <v>22</v>
@@ -8009,9 +8605,12 @@
       <c r="O62" s="7">
         <v>1.0500000000000001E-2</v>
       </c>
-    </row>
-    <row r="63" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A63" s="35"/>
+      <c r="P62" s="44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A63" s="57"/>
       <c r="B63" s="12">
         <v>0.54166666666666696</v>
       </c>
@@ -8040,7 +8639,7 @@
         <v>60</v>
       </c>
       <c r="K63" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L63" s="1">
         <v>22</v>
@@ -8054,9 +8653,12 @@
       <c r="O63" s="7">
         <v>1.0500000000000001E-2</v>
       </c>
-    </row>
-    <row r="64" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A64" s="35"/>
+      <c r="P63" s="44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A64" s="57"/>
       <c r="B64" s="12">
         <v>0.58333333333333304</v>
       </c>
@@ -8085,7 +8687,7 @@
         <v>60</v>
       </c>
       <c r="K64" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L64" s="1">
         <v>22</v>
@@ -8099,9 +8701,12 @@
       <c r="O64" s="7">
         <v>1.0500000000000001E-2</v>
       </c>
-    </row>
-    <row r="65" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A65" s="35"/>
+      <c r="P64" s="44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A65" s="57"/>
       <c r="B65" s="12">
         <v>0.625</v>
       </c>
@@ -8130,7 +8735,7 @@
         <v>60</v>
       </c>
       <c r="K65" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L65" s="1">
         <v>22</v>
@@ -8144,9 +8749,12 @@
       <c r="O65" s="7">
         <v>1.0500000000000001E-2</v>
       </c>
-    </row>
-    <row r="66" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A66" s="35"/>
+      <c r="P65" s="44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A66" s="57"/>
       <c r="B66" s="12">
         <v>0.66666666666666696</v>
       </c>
@@ -8175,7 +8783,7 @@
         <v>60</v>
       </c>
       <c r="K66" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L66" s="1">
         <v>22</v>
@@ -8189,9 +8797,12 @@
       <c r="O66" s="7">
         <v>1.0500000000000001E-2</v>
       </c>
-    </row>
-    <row r="67" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A67" s="35"/>
+      <c r="P66" s="44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A67" s="57"/>
       <c r="B67" s="12">
         <v>0.70833333333333304</v>
       </c>
@@ -8220,7 +8831,7 @@
         <v>60</v>
       </c>
       <c r="K67" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L67" s="1">
         <v>22</v>
@@ -8234,9 +8845,12 @@
       <c r="O67" s="7">
         <v>1.0500000000000001E-2</v>
       </c>
-    </row>
-    <row r="68" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A68" s="35"/>
+      <c r="P67" s="44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A68" s="57"/>
       <c r="B68" s="12">
         <v>0.75</v>
       </c>
@@ -8265,7 +8879,7 @@
         <v>60</v>
       </c>
       <c r="K68" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L68" s="1">
         <v>22</v>
@@ -8279,9 +8893,12 @@
       <c r="O68" s="7">
         <v>1.0500000000000001E-2</v>
       </c>
-    </row>
-    <row r="69" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A69" s="35"/>
+      <c r="P68" s="44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A69" s="57"/>
       <c r="B69" s="12">
         <v>0.79166666666666696</v>
       </c>
@@ -8310,7 +8927,7 @@
         <v>60</v>
       </c>
       <c r="K69" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L69" s="1">
         <v>22</v>
@@ -8324,9 +8941,12 @@
       <c r="O69" s="7">
         <v>1.0500000000000001E-2</v>
       </c>
-    </row>
-    <row r="70" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A70" s="35"/>
+      <c r="P69" s="44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A70" s="57"/>
       <c r="B70" s="12">
         <v>0.83333333333333304</v>
       </c>
@@ -8355,7 +8975,7 @@
         <v>60</v>
       </c>
       <c r="K70" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L70" s="1">
         <v>22</v>
@@ -8369,9 +8989,12 @@
       <c r="O70" s="7">
         <v>1.0500000000000001E-2</v>
       </c>
-    </row>
-    <row r="71" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A71" s="35"/>
+      <c r="P70" s="44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A71" s="57"/>
       <c r="B71" s="12">
         <v>0.875</v>
       </c>
@@ -8400,7 +9023,7 @@
         <v>60</v>
       </c>
       <c r="K71" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L71" s="1">
         <v>22</v>
@@ -8414,9 +9037,12 @@
       <c r="O71" s="7">
         <v>1.0500000000000001E-2</v>
       </c>
-    </row>
-    <row r="72" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A72" s="35"/>
+      <c r="P71" s="44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A72" s="57"/>
       <c r="B72" s="12">
         <v>0.91666666666666696</v>
       </c>
@@ -8445,7 +9071,7 @@
         <v>60</v>
       </c>
       <c r="K72" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L72" s="1">
         <v>22</v>
@@ -8459,9 +9085,12 @@
       <c r="O72" s="7">
         <v>1.0500000000000001E-2</v>
       </c>
-    </row>
-    <row r="73" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A73" s="35"/>
+      <c r="P72" s="44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A73" s="57"/>
       <c r="B73" s="12">
         <v>0.95833333333333304</v>
       </c>
@@ -8490,7 +9119,7 @@
         <v>60</v>
       </c>
       <c r="K73" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L73" s="1">
         <v>22</v>
@@ -8504,9 +9133,12 @@
       <c r="O73" s="7">
         <v>1.0500000000000001E-2</v>
       </c>
-    </row>
-    <row r="74" spans="1:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A74" s="36"/>
+      <c r="P73" s="44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:16" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A74" s="58"/>
       <c r="B74" s="13">
         <v>0.999999999999999</v>
       </c>
@@ -8535,7 +9167,7 @@
         <v>60</v>
       </c>
       <c r="K74" s="8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L74" s="9">
         <v>22</v>
@@ -8548,6 +9180,9 @@
       </c>
       <c r="O74" s="10">
         <v>1.0500000000000001E-2</v>
+      </c>
+      <c r="P74" s="45">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
New unit for DHW (L/(m2 h)
</commit_message>
<xml_diff>
--- a/eureca_ubem/Input/Schedules.xlsx
+++ b/eureca_ubem/Input/Schedules.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pratenr82256\Desktop\eureca-ubem\eureca_ubem\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D507CBBA-9830-4A3C-B8CD-C80371CC68AB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA9F62EB-B757-4A51-AECB-3F6972A985FD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8370" yWindow="0" windowWidth="28800" windowHeight="12225" activeTab="1" xr2:uid="{102ADA3B-B81C-C94C-911C-48E8DF6FFDE7}"/>
+    <workbookView xWindow="10230" yWindow="0" windowWidth="28800" windowHeight="12225" activeTab="1" xr2:uid="{102ADA3B-B81C-C94C-911C-48E8DF6FFDE7}"/>
   </bookViews>
   <sheets>
     <sheet name="GeneralData" sheetId="10" r:id="rId1"/>
@@ -143,9 +143,6 @@
     <t>Domestic Hot Water FlowRate</t>
   </si>
   <si>
-    <t>[L/s]</t>
-  </si>
-  <si>
     <t>DomesticHotWater calculation</t>
   </si>
   <si>
@@ -153,6 +150,9 @@
   </si>
   <si>
     <t>UNI-TS 11300-2</t>
+  </si>
+  <si>
+    <t>[L/(m2 h)]</t>
   </si>
 </sst>
 </file>
@@ -1278,7 +1278,7 @@
         <v>36</v>
       </c>
       <c r="G1" s="49" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J1" s="20" t="s">
         <v>24</v>
@@ -1301,7 +1301,7 @@
         <v>15</v>
       </c>
       <c r="G2" s="46" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J2" t="s">
         <v>25</v>
@@ -1327,7 +1327,7 @@
         <v>1</v>
       </c>
       <c r="G3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
@@ -1369,8 +1369,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE061425-C8E9-4A27-92D2-1582F4E407AA}">
   <dimension ref="A1:AS74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="P51" sqref="P51:P74"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="R14" sqref="R14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1508,7 +1508,7 @@
         <v>27</v>
       </c>
       <c r="P2" s="37" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="Q2" s="16"/>
       <c r="R2" s="16"/>
@@ -1587,7 +1587,7 @@
         <v>1.0500000000000001E-2</v>
       </c>
       <c r="P3" s="43">
-        <v>0.01</v>
+        <v>0</v>
       </c>
       <c r="Q3" s="15"/>
       <c r="R3" s="15"/>
@@ -1664,7 +1664,7 @@
         <v>1.15E-2</v>
       </c>
       <c r="P4" s="44">
-        <v>0.01</v>
+        <v>0</v>
       </c>
       <c r="Q4" s="15"/>
       <c r="R4" s="15"/>
@@ -1741,7 +1741,7 @@
         <v>1.15E-2</v>
       </c>
       <c r="P5" s="44">
-        <v>0.01</v>
+        <v>0</v>
       </c>
       <c r="Q5" s="15"/>
       <c r="R5" s="15"/>
@@ -1818,7 +1818,7 @@
         <v>1.15E-2</v>
       </c>
       <c r="P6" s="44">
-        <v>0.01</v>
+        <v>0</v>
       </c>
       <c r="Q6" s="15"/>
       <c r="R6" s="15"/>
@@ -1895,7 +1895,7 @@
         <v>1.15E-2</v>
       </c>
       <c r="P7" s="44">
-        <v>0.01</v>
+        <v>0</v>
       </c>
       <c r="Q7" s="15"/>
       <c r="R7" s="15"/>
@@ -1972,7 +1972,7 @@
         <v>1.15E-2</v>
       </c>
       <c r="P8" s="44">
-        <v>0.01</v>
+        <v>0</v>
       </c>
       <c r="Q8" s="15"/>
       <c r="R8" s="15"/>
@@ -2049,7 +2049,7 @@
         <v>1.15E-2</v>
       </c>
       <c r="P9" s="44">
-        <v>0.01</v>
+        <v>2.1999999999999999E-2</v>
       </c>
       <c r="Q9" s="15"/>
       <c r="R9" s="15"/>
@@ -2126,7 +2126,7 @@
         <v>1.15E-2</v>
       </c>
       <c r="P10" s="44">
-        <v>0.03</v>
+        <v>2.1999999999999999E-2</v>
       </c>
       <c r="Q10" s="15"/>
       <c r="R10" s="15"/>
@@ -2203,7 +2203,7 @@
         <v>1.15E-2</v>
       </c>
       <c r="P11" s="44">
-        <v>0.03</v>
+        <v>2.1999999999999999E-2</v>
       </c>
     </row>
     <row r="12" spans="1:45" x14ac:dyDescent="0.25">
@@ -2251,7 +2251,7 @@
         <v>1.15E-2</v>
       </c>
       <c r="P12" s="44">
-        <v>0.03</v>
+        <v>2.1999999999999999E-2</v>
       </c>
     </row>
     <row r="13" spans="1:45" x14ac:dyDescent="0.25">
@@ -2299,7 +2299,7 @@
         <v>1.15E-2</v>
       </c>
       <c r="P13" s="44">
-        <v>0.03</v>
+        <v>2.1999999999999999E-2</v>
       </c>
     </row>
     <row r="14" spans="1:45" x14ac:dyDescent="0.25">
@@ -2347,7 +2347,7 @@
         <v>1.15E-2</v>
       </c>
       <c r="P14" s="44">
-        <v>0.03</v>
+        <v>2.1999999999999999E-2</v>
       </c>
     </row>
     <row r="15" spans="1:45" x14ac:dyDescent="0.25">
@@ -2395,7 +2395,7 @@
         <v>1.15E-2</v>
       </c>
       <c r="P15" s="44">
-        <v>0.03</v>
+        <v>2.1999999999999999E-2</v>
       </c>
     </row>
     <row r="16" spans="1:45" x14ac:dyDescent="0.25">
@@ -2443,7 +2443,7 @@
         <v>1.15E-2</v>
       </c>
       <c r="P16" s="44">
-        <v>0.03</v>
+        <v>2.1999999999999999E-2</v>
       </c>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.25">
@@ -2491,7 +2491,7 @@
         <v>1.15E-2</v>
       </c>
       <c r="P17" s="44">
-        <v>0.03</v>
+        <v>2.1999999999999999E-2</v>
       </c>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.25">
@@ -2539,7 +2539,7 @@
         <v>1.15E-2</v>
       </c>
       <c r="P18" s="44">
-        <v>0.03</v>
+        <v>2.1999999999999999E-2</v>
       </c>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.25">
@@ -2587,7 +2587,7 @@
         <v>1.15E-2</v>
       </c>
       <c r="P19" s="44">
-        <v>0.03</v>
+        <v>2.1999999999999999E-2</v>
       </c>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.25">
@@ -2635,7 +2635,7 @@
         <v>1.15E-2</v>
       </c>
       <c r="P20" s="44">
-        <v>0.01</v>
+        <v>2.1999999999999999E-2</v>
       </c>
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.25">
@@ -2683,7 +2683,7 @@
         <v>1.15E-2</v>
       </c>
       <c r="P21" s="44">
-        <v>0.01</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.25">
@@ -2731,7 +2731,7 @@
         <v>1.15E-2</v>
       </c>
       <c r="P22" s="44">
-        <v>0.01</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.25">
@@ -2779,7 +2779,7 @@
         <v>1.15E-2</v>
       </c>
       <c r="P23" s="44">
-        <v>0.01</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.25">
@@ -2827,7 +2827,7 @@
         <v>1.15E-2</v>
       </c>
       <c r="P24" s="44">
-        <v>0.01</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.25">
@@ -2875,7 +2875,7 @@
         <v>1.15E-2</v>
       </c>
       <c r="P25" s="44">
-        <v>0.01</v>
+        <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:16" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -2923,7 +2923,7 @@
         <v>1.15E-2</v>
       </c>
       <c r="P26" s="45">
-        <v>0.01</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.25">
@@ -2976,7 +2976,7 @@
         <v>1.15E-2</v>
       </c>
       <c r="P27" s="43">
-        <v>0.01</v>
+        <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.25">
@@ -3027,7 +3027,7 @@
         <v>1.15E-2</v>
       </c>
       <c r="P28" s="44">
-        <v>0.01</v>
+        <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.25">
@@ -3078,7 +3078,7 @@
         <v>1.15E-2</v>
       </c>
       <c r="P29" s="44">
-        <v>0.01</v>
+        <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.25">
@@ -3129,7 +3129,7 @@
         <v>1.15E-2</v>
       </c>
       <c r="P30" s="44">
-        <v>0.01</v>
+        <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.25">
@@ -3180,7 +3180,7 @@
         <v>1.15E-2</v>
       </c>
       <c r="P31" s="44">
-        <v>0.01</v>
+        <v>0</v>
       </c>
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.25">
@@ -3231,7 +3231,7 @@
         <v>1.15E-2</v>
       </c>
       <c r="P32" s="44">
-        <v>0.01</v>
+        <v>0</v>
       </c>
     </row>
     <row r="33" spans="1:16" x14ac:dyDescent="0.25">
@@ -3282,7 +3282,7 @@
         <v>1.15E-2</v>
       </c>
       <c r="P33" s="44">
-        <v>0.01</v>
+        <v>2.1999999999999999E-2</v>
       </c>
     </row>
     <row r="34" spans="1:16" x14ac:dyDescent="0.25">
@@ -3333,7 +3333,7 @@
         <v>1.15E-2</v>
       </c>
       <c r="P34" s="44">
-        <v>0.03</v>
+        <v>2.1999999999999999E-2</v>
       </c>
     </row>
     <row r="35" spans="1:16" x14ac:dyDescent="0.25">
@@ -3384,7 +3384,7 @@
         <v>1.15E-2</v>
       </c>
       <c r="P35" s="44">
-        <v>0.03</v>
+        <v>2.1999999999999999E-2</v>
       </c>
     </row>
     <row r="36" spans="1:16" x14ac:dyDescent="0.25">
@@ -3435,7 +3435,7 @@
         <v>1.15E-2</v>
       </c>
       <c r="P36" s="44">
-        <v>0.03</v>
+        <v>2.1999999999999999E-2</v>
       </c>
     </row>
     <row r="37" spans="1:16" x14ac:dyDescent="0.25">
@@ -3486,7 +3486,7 @@
         <v>1.15E-2</v>
       </c>
       <c r="P37" s="44">
-        <v>0.03</v>
+        <v>2.1999999999999999E-2</v>
       </c>
     </row>
     <row r="38" spans="1:16" x14ac:dyDescent="0.25">
@@ -3537,7 +3537,7 @@
         <v>1.15E-2</v>
       </c>
       <c r="P38" s="44">
-        <v>0.03</v>
+        <v>2.1999999999999999E-2</v>
       </c>
     </row>
     <row r="39" spans="1:16" x14ac:dyDescent="0.25">
@@ -3588,7 +3588,7 @@
         <v>1.15E-2</v>
       </c>
       <c r="P39" s="44">
-        <v>0.03</v>
+        <v>2.1999999999999999E-2</v>
       </c>
     </row>
     <row r="40" spans="1:16" x14ac:dyDescent="0.25">
@@ -3639,7 +3639,7 @@
         <v>1.15E-2</v>
       </c>
       <c r="P40" s="44">
-        <v>0.03</v>
+        <v>2.1999999999999999E-2</v>
       </c>
     </row>
     <row r="41" spans="1:16" x14ac:dyDescent="0.25">
@@ -3690,7 +3690,7 @@
         <v>1.15E-2</v>
       </c>
       <c r="P41" s="44">
-        <v>0.03</v>
+        <v>2.1999999999999999E-2</v>
       </c>
     </row>
     <row r="42" spans="1:16" x14ac:dyDescent="0.25">
@@ -3741,7 +3741,7 @@
         <v>1.15E-2</v>
       </c>
       <c r="P42" s="44">
-        <v>0.03</v>
+        <v>2.1999999999999999E-2</v>
       </c>
     </row>
     <row r="43" spans="1:16" x14ac:dyDescent="0.25">
@@ -3792,7 +3792,7 @@
         <v>1.15E-2</v>
       </c>
       <c r="P43" s="44">
-        <v>0.03</v>
+        <v>2.1999999999999999E-2</v>
       </c>
     </row>
     <row r="44" spans="1:16" x14ac:dyDescent="0.25">
@@ -3843,7 +3843,7 @@
         <v>1.15E-2</v>
       </c>
       <c r="P44" s="44">
-        <v>0.01</v>
+        <v>2.1999999999999999E-2</v>
       </c>
     </row>
     <row r="45" spans="1:16" x14ac:dyDescent="0.25">
@@ -3894,7 +3894,7 @@
         <v>1.15E-2</v>
       </c>
       <c r="P45" s="44">
-        <v>0.01</v>
+        <v>0</v>
       </c>
     </row>
     <row r="46" spans="1:16" x14ac:dyDescent="0.25">
@@ -3945,7 +3945,7 @@
         <v>1.15E-2</v>
       </c>
       <c r="P46" s="44">
-        <v>0.01</v>
+        <v>0</v>
       </c>
     </row>
     <row r="47" spans="1:16" x14ac:dyDescent="0.25">
@@ -3996,7 +3996,7 @@
         <v>1.15E-2</v>
       </c>
       <c r="P47" s="44">
-        <v>0.01</v>
+        <v>0</v>
       </c>
     </row>
     <row r="48" spans="1:16" x14ac:dyDescent="0.25">
@@ -4047,7 +4047,7 @@
         <v>1.15E-2</v>
       </c>
       <c r="P48" s="44">
-        <v>0.01</v>
+        <v>0</v>
       </c>
     </row>
     <row r="49" spans="1:16" x14ac:dyDescent="0.25">
@@ -4098,7 +4098,7 @@
         <v>1.15E-2</v>
       </c>
       <c r="P49" s="44">
-        <v>0.01</v>
+        <v>0</v>
       </c>
     </row>
     <row r="50" spans="1:16" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -4149,7 +4149,7 @@
         <v>1.15E-2</v>
       </c>
       <c r="P50" s="45">
-        <v>0.01</v>
+        <v>0</v>
       </c>
     </row>
     <row r="51" spans="1:16" x14ac:dyDescent="0.25">
@@ -4199,7 +4199,7 @@
         <v>1.15E-2</v>
       </c>
       <c r="P51" s="43">
-        <v>0.01</v>
+        <v>0</v>
       </c>
     </row>
     <row r="52" spans="1:16" x14ac:dyDescent="0.25">
@@ -4247,7 +4247,7 @@
         <v>1.15E-2</v>
       </c>
       <c r="P52" s="44">
-        <v>0.01</v>
+        <v>0</v>
       </c>
     </row>
     <row r="53" spans="1:16" x14ac:dyDescent="0.25">
@@ -4295,7 +4295,7 @@
         <v>1.15E-2</v>
       </c>
       <c r="P53" s="44">
-        <v>0.01</v>
+        <v>0</v>
       </c>
     </row>
     <row r="54" spans="1:16" x14ac:dyDescent="0.25">
@@ -4343,7 +4343,7 @@
         <v>1.15E-2</v>
       </c>
       <c r="P54" s="44">
-        <v>0.01</v>
+        <v>0</v>
       </c>
     </row>
     <row r="55" spans="1:16" x14ac:dyDescent="0.25">
@@ -4391,7 +4391,7 @@
         <v>1.15E-2</v>
       </c>
       <c r="P55" s="44">
-        <v>0.01</v>
+        <v>0</v>
       </c>
     </row>
     <row r="56" spans="1:16" x14ac:dyDescent="0.25">
@@ -4439,7 +4439,7 @@
         <v>1.15E-2</v>
       </c>
       <c r="P56" s="44">
-        <v>0.01</v>
+        <v>0</v>
       </c>
     </row>
     <row r="57" spans="1:16" x14ac:dyDescent="0.25">
@@ -4487,7 +4487,7 @@
         <v>1.15E-2</v>
       </c>
       <c r="P57" s="44">
-        <v>0.01</v>
+        <v>2.1999999999999999E-2</v>
       </c>
     </row>
     <row r="58" spans="1:16" x14ac:dyDescent="0.25">
@@ -4535,7 +4535,7 @@
         <v>1.15E-2</v>
       </c>
       <c r="P58" s="44">
-        <v>0.03</v>
+        <v>2.1999999999999999E-2</v>
       </c>
     </row>
     <row r="59" spans="1:16" x14ac:dyDescent="0.25">
@@ -4583,7 +4583,7 @@
         <v>1.15E-2</v>
       </c>
       <c r="P59" s="44">
-        <v>0.03</v>
+        <v>2.1999999999999999E-2</v>
       </c>
     </row>
     <row r="60" spans="1:16" x14ac:dyDescent="0.25">
@@ -4631,7 +4631,7 @@
         <v>1.15E-2</v>
       </c>
       <c r="P60" s="44">
-        <v>0.03</v>
+        <v>2.1999999999999999E-2</v>
       </c>
     </row>
     <row r="61" spans="1:16" x14ac:dyDescent="0.25">
@@ -4679,7 +4679,7 @@
         <v>1.15E-2</v>
       </c>
       <c r="P61" s="44">
-        <v>0.03</v>
+        <v>2.1999999999999999E-2</v>
       </c>
     </row>
     <row r="62" spans="1:16" x14ac:dyDescent="0.25">
@@ -4727,7 +4727,7 @@
         <v>1.15E-2</v>
       </c>
       <c r="P62" s="44">
-        <v>0.03</v>
+        <v>2.1999999999999999E-2</v>
       </c>
     </row>
     <row r="63" spans="1:16" x14ac:dyDescent="0.25">
@@ -4775,7 +4775,7 @@
         <v>1.15E-2</v>
       </c>
       <c r="P63" s="44">
-        <v>0.03</v>
+        <v>2.1999999999999999E-2</v>
       </c>
     </row>
     <row r="64" spans="1:16" x14ac:dyDescent="0.25">
@@ -4823,7 +4823,7 @@
         <v>1.15E-2</v>
       </c>
       <c r="P64" s="44">
-        <v>0.03</v>
+        <v>2.1999999999999999E-2</v>
       </c>
     </row>
     <row r="65" spans="1:16" x14ac:dyDescent="0.25">
@@ -4871,7 +4871,7 @@
         <v>1.15E-2</v>
       </c>
       <c r="P65" s="44">
-        <v>0.03</v>
+        <v>2.1999999999999999E-2</v>
       </c>
     </row>
     <row r="66" spans="1:16" x14ac:dyDescent="0.25">
@@ -4919,7 +4919,7 @@
         <v>1.15E-2</v>
       </c>
       <c r="P66" s="44">
-        <v>0.03</v>
+        <v>2.1999999999999999E-2</v>
       </c>
     </row>
     <row r="67" spans="1:16" x14ac:dyDescent="0.25">
@@ -4967,7 +4967,7 @@
         <v>1.15E-2</v>
       </c>
       <c r="P67" s="44">
-        <v>0.03</v>
+        <v>2.1999999999999999E-2</v>
       </c>
     </row>
     <row r="68" spans="1:16" x14ac:dyDescent="0.25">
@@ -5015,7 +5015,7 @@
         <v>1.15E-2</v>
       </c>
       <c r="P68" s="44">
-        <v>0.01</v>
+        <v>2.1999999999999999E-2</v>
       </c>
     </row>
     <row r="69" spans="1:16" x14ac:dyDescent="0.25">
@@ -5063,7 +5063,7 @@
         <v>1.15E-2</v>
       </c>
       <c r="P69" s="44">
-        <v>0.01</v>
+        <v>0</v>
       </c>
     </row>
     <row r="70" spans="1:16" x14ac:dyDescent="0.25">
@@ -5111,7 +5111,7 @@
         <v>1.15E-2</v>
       </c>
       <c r="P70" s="44">
-        <v>0.01</v>
+        <v>0</v>
       </c>
     </row>
     <row r="71" spans="1:16" x14ac:dyDescent="0.25">
@@ -5159,7 +5159,7 @@
         <v>1.15E-2</v>
       </c>
       <c r="P71" s="44">
-        <v>0.01</v>
+        <v>0</v>
       </c>
     </row>
     <row r="72" spans="1:16" x14ac:dyDescent="0.25">
@@ -5207,7 +5207,7 @@
         <v>1.15E-2</v>
       </c>
       <c r="P72" s="44">
-        <v>0.01</v>
+        <v>0</v>
       </c>
     </row>
     <row r="73" spans="1:16" x14ac:dyDescent="0.25">
@@ -5255,7 +5255,7 @@
         <v>1.15E-2</v>
       </c>
       <c r="P73" s="44">
-        <v>0.01</v>
+        <v>0</v>
       </c>
     </row>
     <row r="74" spans="1:16" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -5303,7 +5303,7 @@
         <v>1.15E-2</v>
       </c>
       <c r="P74" s="45">
-        <v>0.01</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -5321,7 +5321,7 @@
   <dimension ref="A1:AS74"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="P3" sqref="P3"/>
+      <selection activeCell="O15" sqref="O15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -5459,7 +5459,7 @@
         <v>27</v>
       </c>
       <c r="P2" s="37" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="Q2" s="16"/>
       <c r="R2" s="16"/>

</xml_diff>

<commit_message>
New option in schedules excel for stochatstic italian electri loads
</commit_message>
<xml_diff>
--- a/eureca_ubem/Input/Schedules.xlsx
+++ b/eureca_ubem/Input/Schedules.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20398"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20401"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pratenr82256\Desktop\eureca-ubem\eureca_ubem\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA9F62EB-B757-4A51-AECB-3F6972A985FD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DE27ED6-BA58-4CBC-9D18-4600C66EBFC7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10230" yWindow="0" windowWidth="28800" windowHeight="12225" activeTab="1" xr2:uid="{102ADA3B-B81C-C94C-911C-48E8DF6FFDE7}"/>
+    <workbookView xWindow="13020" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{102ADA3B-B81C-C94C-911C-48E8DF6FFDE7}"/>
   </bookViews>
   <sheets>
     <sheet name="GeneralData" sheetId="10" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="44">
   <si>
     <t>Weekday</t>
   </si>
@@ -154,6 +154,12 @@
   <si>
     <t>[L/(m2 h)]</t>
   </si>
+  <si>
+    <t>Appliances calculation</t>
+  </si>
+  <si>
+    <t>Italian Residential Building Stock</t>
+  </si>
 </sst>
 </file>
 
@@ -171,7 +177,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -238,6 +244,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor rgb="FFA9D18E"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="32">
     <border>
@@ -678,7 +696,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -819,6 +837,10 @@
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1242,8 +1264,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76CB4D20-8171-4D3A-B436-C3966BA8F7D8}">
   <dimension ref="A1:J4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1255,6 +1277,7 @@
     <col min="5" max="5" width="12.5" customWidth="1"/>
     <col min="6" max="6" width="12" customWidth="1"/>
     <col min="7" max="7" width="17.5" customWidth="1"/>
+    <col min="8" max="8" width="16.625" customWidth="1"/>
     <col min="10" max="10" width="14.375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1280,6 +1303,9 @@
       <c r="G1" s="49" t="s">
         <v>38</v>
       </c>
+      <c r="H1" s="50" t="s">
+        <v>42</v>
+      </c>
       <c r="J1" s="20" t="s">
         <v>24</v>
       </c>
@@ -1303,6 +1329,9 @@
       <c r="G2" s="46" t="s">
         <v>39</v>
       </c>
+      <c r="H2" s="51" t="s">
+        <v>39</v>
+      </c>
       <c r="J2" t="s">
         <v>25</v>
       </c>
@@ -1328,6 +1357,9 @@
       </c>
       <c r="G3" t="s">
         <v>40</v>
+      </c>
+      <c r="H3" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
@@ -1352,11 +1384,17 @@
       <c r="G4" t="s">
         <v>20</v>
       </c>
+      <c r="H4" t="s">
+        <v>20</v>
+      </c>
     </row>
   </sheetData>
-  <dataValidations count="1">
+  <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G3:G105" xr:uid="{8D8140ED-8C4A-489F-8C7E-0BC81CB30031}">
       <formula1>"Schedule,UNI-TS 11300-2"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H3:H1048576" xr:uid="{B24BD31C-DC54-4FED-B50C-B59BE5740BCD}">
+      <formula1>"Schedule,Italian Residential Building Stock"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1369,7 +1407,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE061425-C8E9-4A27-92D2-1582F4E407AA}">
   <dimension ref="A1:AS74"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="R14" sqref="R14"/>
     </sheetView>
   </sheetViews>
@@ -1541,7 +1579,7 @@
       <c r="AS2" s="15"/>
     </row>
     <row r="3" spans="1:45" x14ac:dyDescent="0.25">
-      <c r="A3" s="50" t="s">
+      <c r="A3" s="52" t="s">
         <v>0</v>
       </c>
       <c r="B3" s="11">
@@ -1620,7 +1658,7 @@
       <c r="AS3" s="15"/>
     </row>
     <row r="4" spans="1:45" x14ac:dyDescent="0.25">
-      <c r="A4" s="51"/>
+      <c r="A4" s="53"/>
       <c r="B4" s="12">
         <v>8.3333333333333301E-2</v>
       </c>
@@ -1697,7 +1735,7 @@
       <c r="AS4" s="15"/>
     </row>
     <row r="5" spans="1:45" x14ac:dyDescent="0.25">
-      <c r="A5" s="51"/>
+      <c r="A5" s="53"/>
       <c r="B5" s="12">
         <v>0.125</v>
       </c>
@@ -1774,7 +1812,7 @@
       <c r="AS5" s="15"/>
     </row>
     <row r="6" spans="1:45" x14ac:dyDescent="0.25">
-      <c r="A6" s="51"/>
+      <c r="A6" s="53"/>
       <c r="B6" s="12">
         <v>0.16666666666666699</v>
       </c>
@@ -1851,7 +1889,7 @@
       <c r="AS6" s="15"/>
     </row>
     <row r="7" spans="1:45" x14ac:dyDescent="0.25">
-      <c r="A7" s="51"/>
+      <c r="A7" s="53"/>
       <c r="B7" s="12">
         <v>0.20833333333333301</v>
       </c>
@@ -1928,7 +1966,7 @@
       <c r="AS7" s="15"/>
     </row>
     <row r="8" spans="1:45" x14ac:dyDescent="0.25">
-      <c r="A8" s="51"/>
+      <c r="A8" s="53"/>
       <c r="B8" s="12">
         <v>0.25</v>
       </c>
@@ -2005,7 +2043,7 @@
       <c r="AS8" s="15"/>
     </row>
     <row r="9" spans="1:45" x14ac:dyDescent="0.25">
-      <c r="A9" s="51"/>
+      <c r="A9" s="53"/>
       <c r="B9" s="12">
         <v>0.29166666666666702</v>
       </c>
@@ -2082,7 +2120,7 @@
       <c r="AS9" s="15"/>
     </row>
     <row r="10" spans="1:45" x14ac:dyDescent="0.25">
-      <c r="A10" s="51"/>
+      <c r="A10" s="53"/>
       <c r="B10" s="12">
         <v>0.33333333333333298</v>
       </c>
@@ -2159,7 +2197,7 @@
       <c r="AS10" s="15"/>
     </row>
     <row r="11" spans="1:45" x14ac:dyDescent="0.25">
-      <c r="A11" s="51"/>
+      <c r="A11" s="53"/>
       <c r="B11" s="12">
         <v>0.375</v>
       </c>
@@ -2207,7 +2245,7 @@
       </c>
     </row>
     <row r="12" spans="1:45" x14ac:dyDescent="0.25">
-      <c r="A12" s="51"/>
+      <c r="A12" s="53"/>
       <c r="B12" s="12">
         <v>0.41666666666666702</v>
       </c>
@@ -2255,7 +2293,7 @@
       </c>
     </row>
     <row r="13" spans="1:45" x14ac:dyDescent="0.25">
-      <c r="A13" s="51"/>
+      <c r="A13" s="53"/>
       <c r="B13" s="12">
         <v>0.45833333333333298</v>
       </c>
@@ -2303,7 +2341,7 @@
       </c>
     </row>
     <row r="14" spans="1:45" x14ac:dyDescent="0.25">
-      <c r="A14" s="51"/>
+      <c r="A14" s="53"/>
       <c r="B14" s="12">
         <v>0.5</v>
       </c>
@@ -2351,7 +2389,7 @@
       </c>
     </row>
     <row r="15" spans="1:45" x14ac:dyDescent="0.25">
-      <c r="A15" s="51"/>
+      <c r="A15" s="53"/>
       <c r="B15" s="12">
         <v>0.54166666666666696</v>
       </c>
@@ -2399,7 +2437,7 @@
       </c>
     </row>
     <row r="16" spans="1:45" x14ac:dyDescent="0.25">
-      <c r="A16" s="51"/>
+      <c r="A16" s="53"/>
       <c r="B16" s="12">
         <v>0.58333333333333304</v>
       </c>
@@ -2447,7 +2485,7 @@
       </c>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A17" s="51"/>
+      <c r="A17" s="53"/>
       <c r="B17" s="12">
         <v>0.625</v>
       </c>
@@ -2495,7 +2533,7 @@
       </c>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A18" s="51"/>
+      <c r="A18" s="53"/>
       <c r="B18" s="12">
         <v>0.66666666666666696</v>
       </c>
@@ -2543,7 +2581,7 @@
       </c>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A19" s="51"/>
+      <c r="A19" s="53"/>
       <c r="B19" s="12">
         <v>0.70833333333333304</v>
       </c>
@@ -2591,7 +2629,7 @@
       </c>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A20" s="51"/>
+      <c r="A20" s="53"/>
       <c r="B20" s="12">
         <v>0.75</v>
       </c>
@@ -2639,7 +2677,7 @@
       </c>
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A21" s="51"/>
+      <c r="A21" s="53"/>
       <c r="B21" s="12">
         <v>0.79166666666666696</v>
       </c>
@@ -2687,7 +2725,7 @@
       </c>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A22" s="51"/>
+      <c r="A22" s="53"/>
       <c r="B22" s="12">
         <v>0.83333333333333304</v>
       </c>
@@ -2735,7 +2773,7 @@
       </c>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A23" s="51"/>
+      <c r="A23" s="53"/>
       <c r="B23" s="12">
         <v>0.875</v>
       </c>
@@ -2783,7 +2821,7 @@
       </c>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A24" s="51"/>
+      <c r="A24" s="53"/>
       <c r="B24" s="12">
         <v>0.91666666666666696</v>
       </c>
@@ -2831,7 +2869,7 @@
       </c>
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A25" s="51"/>
+      <c r="A25" s="53"/>
       <c r="B25" s="12">
         <v>0.95833333333333304</v>
       </c>
@@ -2879,7 +2917,7 @@
       </c>
     </row>
     <row r="26" spans="1:16" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="52"/>
+      <c r="A26" s="54"/>
       <c r="B26" s="13">
         <v>0.999999999999999</v>
       </c>
@@ -2927,7 +2965,7 @@
       </c>
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A27" s="53" t="s">
+      <c r="A27" s="55" t="s">
         <v>18</v>
       </c>
       <c r="B27" s="11">
@@ -2980,7 +3018,7 @@
       </c>
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A28" s="54"/>
+      <c r="A28" s="56"/>
       <c r="B28" s="12">
         <v>8.3333333333333301E-2</v>
       </c>
@@ -3031,7 +3069,7 @@
       </c>
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A29" s="54"/>
+      <c r="A29" s="56"/>
       <c r="B29" s="12">
         <v>0.125</v>
       </c>
@@ -3082,7 +3120,7 @@
       </c>
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A30" s="54"/>
+      <c r="A30" s="56"/>
       <c r="B30" s="12">
         <v>0.16666666666666699</v>
       </c>
@@ -3133,7 +3171,7 @@
       </c>
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A31" s="54"/>
+      <c r="A31" s="56"/>
       <c r="B31" s="12">
         <v>0.20833333333333301</v>
       </c>
@@ -3184,7 +3222,7 @@
       </c>
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A32" s="54"/>
+      <c r="A32" s="56"/>
       <c r="B32" s="12">
         <v>0.25</v>
       </c>
@@ -3235,7 +3273,7 @@
       </c>
     </row>
     <row r="33" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A33" s="54"/>
+      <c r="A33" s="56"/>
       <c r="B33" s="12">
         <v>0.29166666666666702</v>
       </c>
@@ -3286,7 +3324,7 @@
       </c>
     </row>
     <row r="34" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A34" s="54"/>
+      <c r="A34" s="56"/>
       <c r="B34" s="12">
         <v>0.33333333333333298</v>
       </c>
@@ -3337,7 +3375,7 @@
       </c>
     </row>
     <row r="35" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A35" s="54"/>
+      <c r="A35" s="56"/>
       <c r="B35" s="12">
         <v>0.375</v>
       </c>
@@ -3388,7 +3426,7 @@
       </c>
     </row>
     <row r="36" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A36" s="54"/>
+      <c r="A36" s="56"/>
       <c r="B36" s="12">
         <v>0.41666666666666702</v>
       </c>
@@ -3439,7 +3477,7 @@
       </c>
     </row>
     <row r="37" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A37" s="54"/>
+      <c r="A37" s="56"/>
       <c r="B37" s="12">
         <v>0.45833333333333298</v>
       </c>
@@ -3490,7 +3528,7 @@
       </c>
     </row>
     <row r="38" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A38" s="54"/>
+      <c r="A38" s="56"/>
       <c r="B38" s="12">
         <v>0.5</v>
       </c>
@@ -3541,7 +3579,7 @@
       </c>
     </row>
     <row r="39" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A39" s="54"/>
+      <c r="A39" s="56"/>
       <c r="B39" s="12">
         <v>0.54166666666666696</v>
       </c>
@@ -3592,7 +3630,7 @@
       </c>
     </row>
     <row r="40" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A40" s="54"/>
+      <c r="A40" s="56"/>
       <c r="B40" s="12">
         <v>0.58333333333333304</v>
       </c>
@@ -3643,7 +3681,7 @@
       </c>
     </row>
     <row r="41" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A41" s="54"/>
+      <c r="A41" s="56"/>
       <c r="B41" s="12">
         <v>0.625</v>
       </c>
@@ -3694,7 +3732,7 @@
       </c>
     </row>
     <row r="42" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A42" s="54"/>
+      <c r="A42" s="56"/>
       <c r="B42" s="12">
         <v>0.66666666666666696</v>
       </c>
@@ -3745,7 +3783,7 @@
       </c>
     </row>
     <row r="43" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A43" s="54"/>
+      <c r="A43" s="56"/>
       <c r="B43" s="12">
         <v>0.70833333333333304</v>
       </c>
@@ -3796,7 +3834,7 @@
       </c>
     </row>
     <row r="44" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A44" s="54"/>
+      <c r="A44" s="56"/>
       <c r="B44" s="12">
         <v>0.75</v>
       </c>
@@ -3847,7 +3885,7 @@
       </c>
     </row>
     <row r="45" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A45" s="54"/>
+      <c r="A45" s="56"/>
       <c r="B45" s="12">
         <v>0.79166666666666696</v>
       </c>
@@ -3898,7 +3936,7 @@
       </c>
     </row>
     <row r="46" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A46" s="54"/>
+      <c r="A46" s="56"/>
       <c r="B46" s="12">
         <v>0.83333333333333304</v>
       </c>
@@ -3949,7 +3987,7 @@
       </c>
     </row>
     <row r="47" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A47" s="54"/>
+      <c r="A47" s="56"/>
       <c r="B47" s="12">
         <v>0.875</v>
       </c>
@@ -4000,7 +4038,7 @@
       </c>
     </row>
     <row r="48" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A48" s="54"/>
+      <c r="A48" s="56"/>
       <c r="B48" s="12">
         <v>0.91666666666666696</v>
       </c>
@@ -4051,7 +4089,7 @@
       </c>
     </row>
     <row r="49" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A49" s="54"/>
+      <c r="A49" s="56"/>
       <c r="B49" s="12">
         <v>0.95833333333333304</v>
       </c>
@@ -4102,7 +4140,7 @@
       </c>
     </row>
     <row r="50" spans="1:16" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="55"/>
+      <c r="A50" s="57"/>
       <c r="B50" s="13">
         <v>0.999999999999999</v>
       </c>
@@ -4153,7 +4191,7 @@
       </c>
     </row>
     <row r="51" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A51" s="56" t="s">
+      <c r="A51" s="58" t="s">
         <v>19</v>
       </c>
       <c r="B51" s="11">
@@ -4203,7 +4241,7 @@
       </c>
     </row>
     <row r="52" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A52" s="57"/>
+      <c r="A52" s="59"/>
       <c r="B52" s="12">
         <v>8.3333333333333301E-2</v>
       </c>
@@ -4251,7 +4289,7 @@
       </c>
     </row>
     <row r="53" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A53" s="57"/>
+      <c r="A53" s="59"/>
       <c r="B53" s="12">
         <v>0.125</v>
       </c>
@@ -4299,7 +4337,7 @@
       </c>
     </row>
     <row r="54" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A54" s="57"/>
+      <c r="A54" s="59"/>
       <c r="B54" s="12">
         <v>0.16666666666666699</v>
       </c>
@@ -4347,7 +4385,7 @@
       </c>
     </row>
     <row r="55" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A55" s="57"/>
+      <c r="A55" s="59"/>
       <c r="B55" s="12">
         <v>0.20833333333333301</v>
       </c>
@@ -4395,7 +4433,7 @@
       </c>
     </row>
     <row r="56" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A56" s="57"/>
+      <c r="A56" s="59"/>
       <c r="B56" s="12">
         <v>0.25</v>
       </c>
@@ -4443,7 +4481,7 @@
       </c>
     </row>
     <row r="57" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A57" s="57"/>
+      <c r="A57" s="59"/>
       <c r="B57" s="12">
         <v>0.29166666666666702</v>
       </c>
@@ -4491,7 +4529,7 @@
       </c>
     </row>
     <row r="58" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A58" s="57"/>
+      <c r="A58" s="59"/>
       <c r="B58" s="12">
         <v>0.33333333333333298</v>
       </c>
@@ -4539,7 +4577,7 @@
       </c>
     </row>
     <row r="59" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A59" s="57"/>
+      <c r="A59" s="59"/>
       <c r="B59" s="12">
         <v>0.375</v>
       </c>
@@ -4587,7 +4625,7 @@
       </c>
     </row>
     <row r="60" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A60" s="57"/>
+      <c r="A60" s="59"/>
       <c r="B60" s="12">
         <v>0.41666666666666702</v>
       </c>
@@ -4635,7 +4673,7 @@
       </c>
     </row>
     <row r="61" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A61" s="57"/>
+      <c r="A61" s="59"/>
       <c r="B61" s="12">
         <v>0.45833333333333298</v>
       </c>
@@ -4683,7 +4721,7 @@
       </c>
     </row>
     <row r="62" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A62" s="57"/>
+      <c r="A62" s="59"/>
       <c r="B62" s="12">
         <v>0.5</v>
       </c>
@@ -4731,7 +4769,7 @@
       </c>
     </row>
     <row r="63" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A63" s="57"/>
+      <c r="A63" s="59"/>
       <c r="B63" s="12">
         <v>0.54166666666666696</v>
       </c>
@@ -4779,7 +4817,7 @@
       </c>
     </row>
     <row r="64" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A64" s="57"/>
+      <c r="A64" s="59"/>
       <c r="B64" s="12">
         <v>0.58333333333333304</v>
       </c>
@@ -4827,7 +4865,7 @@
       </c>
     </row>
     <row r="65" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A65" s="57"/>
+      <c r="A65" s="59"/>
       <c r="B65" s="12">
         <v>0.625</v>
       </c>
@@ -4875,7 +4913,7 @@
       </c>
     </row>
     <row r="66" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A66" s="57"/>
+      <c r="A66" s="59"/>
       <c r="B66" s="12">
         <v>0.66666666666666696</v>
       </c>
@@ -4923,7 +4961,7 @@
       </c>
     </row>
     <row r="67" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A67" s="57"/>
+      <c r="A67" s="59"/>
       <c r="B67" s="12">
         <v>0.70833333333333304</v>
       </c>
@@ -4971,7 +5009,7 @@
       </c>
     </row>
     <row r="68" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A68" s="57"/>
+      <c r="A68" s="59"/>
       <c r="B68" s="12">
         <v>0.75</v>
       </c>
@@ -5019,7 +5057,7 @@
       </c>
     </row>
     <row r="69" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A69" s="57"/>
+      <c r="A69" s="59"/>
       <c r="B69" s="12">
         <v>0.79166666666666696</v>
       </c>
@@ -5067,7 +5105,7 @@
       </c>
     </row>
     <row r="70" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A70" s="57"/>
+      <c r="A70" s="59"/>
       <c r="B70" s="12">
         <v>0.83333333333333304</v>
       </c>
@@ -5115,7 +5153,7 @@
       </c>
     </row>
     <row r="71" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A71" s="57"/>
+      <c r="A71" s="59"/>
       <c r="B71" s="12">
         <v>0.875</v>
       </c>
@@ -5163,7 +5201,7 @@
       </c>
     </row>
     <row r="72" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A72" s="57"/>
+      <c r="A72" s="59"/>
       <c r="B72" s="12">
         <v>0.91666666666666696</v>
       </c>
@@ -5211,7 +5249,7 @@
       </c>
     </row>
     <row r="73" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A73" s="57"/>
+      <c r="A73" s="59"/>
       <c r="B73" s="12">
         <v>0.95833333333333304</v>
       </c>
@@ -5259,7 +5297,7 @@
       </c>
     </row>
     <row r="74" spans="1:16" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A74" s="58"/>
+      <c r="A74" s="60"/>
       <c r="B74" s="13">
         <v>0.999999999999999</v>
       </c>
@@ -5492,7 +5530,7 @@
       <c r="AS2" s="15"/>
     </row>
     <row r="3" spans="1:45" x14ac:dyDescent="0.25">
-      <c r="A3" s="50" t="s">
+      <c r="A3" s="52" t="s">
         <v>0</v>
       </c>
       <c r="B3" s="11">
@@ -5571,7 +5609,7 @@
       <c r="AS3" s="15"/>
     </row>
     <row r="4" spans="1:45" x14ac:dyDescent="0.25">
-      <c r="A4" s="51"/>
+      <c r="A4" s="53"/>
       <c r="B4" s="12">
         <v>8.3333333333333301E-2</v>
       </c>
@@ -5648,7 +5686,7 @@
       <c r="AS4" s="15"/>
     </row>
     <row r="5" spans="1:45" x14ac:dyDescent="0.25">
-      <c r="A5" s="51"/>
+      <c r="A5" s="53"/>
       <c r="B5" s="12">
         <v>0.125</v>
       </c>
@@ -5725,7 +5763,7 @@
       <c r="AS5" s="15"/>
     </row>
     <row r="6" spans="1:45" x14ac:dyDescent="0.25">
-      <c r="A6" s="51"/>
+      <c r="A6" s="53"/>
       <c r="B6" s="12">
         <v>0.16666666666666699</v>
       </c>
@@ -5802,7 +5840,7 @@
       <c r="AS6" s="15"/>
     </row>
     <row r="7" spans="1:45" x14ac:dyDescent="0.25">
-      <c r="A7" s="51"/>
+      <c r="A7" s="53"/>
       <c r="B7" s="12">
         <v>0.20833333333333301</v>
       </c>
@@ -5879,7 +5917,7 @@
       <c r="AS7" s="15"/>
     </row>
     <row r="8" spans="1:45" x14ac:dyDescent="0.25">
-      <c r="A8" s="51"/>
+      <c r="A8" s="53"/>
       <c r="B8" s="12">
         <v>0.25</v>
       </c>
@@ -5956,7 +5994,7 @@
       <c r="AS8" s="15"/>
     </row>
     <row r="9" spans="1:45" x14ac:dyDescent="0.25">
-      <c r="A9" s="51"/>
+      <c r="A9" s="53"/>
       <c r="B9" s="12">
         <v>0.29166666666666702</v>
       </c>
@@ -6033,7 +6071,7 @@
       <c r="AS9" s="15"/>
     </row>
     <row r="10" spans="1:45" x14ac:dyDescent="0.25">
-      <c r="A10" s="51"/>
+      <c r="A10" s="53"/>
       <c r="B10" s="12">
         <v>0.33333333333333298</v>
       </c>
@@ -6110,7 +6148,7 @@
       <c r="AS10" s="15"/>
     </row>
     <row r="11" spans="1:45" x14ac:dyDescent="0.25">
-      <c r="A11" s="51"/>
+      <c r="A11" s="53"/>
       <c r="B11" s="12">
         <v>0.375</v>
       </c>
@@ -6158,7 +6196,7 @@
       </c>
     </row>
     <row r="12" spans="1:45" x14ac:dyDescent="0.25">
-      <c r="A12" s="51"/>
+      <c r="A12" s="53"/>
       <c r="B12" s="12">
         <v>0.41666666666666702</v>
       </c>
@@ -6206,7 +6244,7 @@
       </c>
     </row>
     <row r="13" spans="1:45" x14ac:dyDescent="0.25">
-      <c r="A13" s="51"/>
+      <c r="A13" s="53"/>
       <c r="B13" s="12">
         <v>0.45833333333333298</v>
       </c>
@@ -6254,7 +6292,7 @@
       </c>
     </row>
     <row r="14" spans="1:45" x14ac:dyDescent="0.25">
-      <c r="A14" s="51"/>
+      <c r="A14" s="53"/>
       <c r="B14" s="12">
         <v>0.5</v>
       </c>
@@ -6302,7 +6340,7 @@
       </c>
     </row>
     <row r="15" spans="1:45" x14ac:dyDescent="0.25">
-      <c r="A15" s="51"/>
+      <c r="A15" s="53"/>
       <c r="B15" s="12">
         <v>0.54166666666666696</v>
       </c>
@@ -6350,7 +6388,7 @@
       </c>
     </row>
     <row r="16" spans="1:45" x14ac:dyDescent="0.25">
-      <c r="A16" s="51"/>
+      <c r="A16" s="53"/>
       <c r="B16" s="12">
         <v>0.58333333333333304</v>
       </c>
@@ -6398,7 +6436,7 @@
       </c>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A17" s="51"/>
+      <c r="A17" s="53"/>
       <c r="B17" s="12">
         <v>0.625</v>
       </c>
@@ -6446,7 +6484,7 @@
       </c>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A18" s="51"/>
+      <c r="A18" s="53"/>
       <c r="B18" s="12">
         <v>0.66666666666666696</v>
       </c>
@@ -6494,7 +6532,7 @@
       </c>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A19" s="51"/>
+      <c r="A19" s="53"/>
       <c r="B19" s="12">
         <v>0.70833333333333304</v>
       </c>
@@ -6542,7 +6580,7 @@
       </c>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A20" s="51"/>
+      <c r="A20" s="53"/>
       <c r="B20" s="12">
         <v>0.75</v>
       </c>
@@ -6590,7 +6628,7 @@
       </c>
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A21" s="51"/>
+      <c r="A21" s="53"/>
       <c r="B21" s="12">
         <v>0.79166666666666696</v>
       </c>
@@ -6638,7 +6676,7 @@
       </c>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A22" s="51"/>
+      <c r="A22" s="53"/>
       <c r="B22" s="12">
         <v>0.83333333333333304</v>
       </c>
@@ -6686,7 +6724,7 @@
       </c>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A23" s="51"/>
+      <c r="A23" s="53"/>
       <c r="B23" s="12">
         <v>0.875</v>
       </c>
@@ -6734,7 +6772,7 @@
       </c>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A24" s="51"/>
+      <c r="A24" s="53"/>
       <c r="B24" s="12">
         <v>0.91666666666666696</v>
       </c>
@@ -6782,7 +6820,7 @@
       </c>
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A25" s="51"/>
+      <c r="A25" s="53"/>
       <c r="B25" s="12">
         <v>0.95833333333333304</v>
       </c>
@@ -6830,7 +6868,7 @@
       </c>
     </row>
     <row r="26" spans="1:16" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="52"/>
+      <c r="A26" s="54"/>
       <c r="B26" s="13">
         <v>0.999999999999999</v>
       </c>
@@ -6878,7 +6916,7 @@
       </c>
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A27" s="53" t="s">
+      <c r="A27" s="55" t="s">
         <v>18</v>
       </c>
       <c r="B27" s="11">
@@ -6928,7 +6966,7 @@
       </c>
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A28" s="54"/>
+      <c r="A28" s="56"/>
       <c r="B28" s="12">
         <v>8.3333333333333301E-2</v>
       </c>
@@ -6976,7 +7014,7 @@
       </c>
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A29" s="54"/>
+      <c r="A29" s="56"/>
       <c r="B29" s="12">
         <v>0.125</v>
       </c>
@@ -7024,7 +7062,7 @@
       </c>
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A30" s="54"/>
+      <c r="A30" s="56"/>
       <c r="B30" s="12">
         <v>0.16666666666666699</v>
       </c>
@@ -7072,7 +7110,7 @@
       </c>
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A31" s="54"/>
+      <c r="A31" s="56"/>
       <c r="B31" s="12">
         <v>0.20833333333333301</v>
       </c>
@@ -7120,7 +7158,7 @@
       </c>
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A32" s="54"/>
+      <c r="A32" s="56"/>
       <c r="B32" s="12">
         <v>0.25</v>
       </c>
@@ -7168,7 +7206,7 @@
       </c>
     </row>
     <row r="33" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A33" s="54"/>
+      <c r="A33" s="56"/>
       <c r="B33" s="12">
         <v>0.29166666666666702</v>
       </c>
@@ -7216,7 +7254,7 @@
       </c>
     </row>
     <row r="34" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A34" s="54"/>
+      <c r="A34" s="56"/>
       <c r="B34" s="12">
         <v>0.33333333333333298</v>
       </c>
@@ -7264,7 +7302,7 @@
       </c>
     </row>
     <row r="35" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A35" s="54"/>
+      <c r="A35" s="56"/>
       <c r="B35" s="12">
         <v>0.375</v>
       </c>
@@ -7312,7 +7350,7 @@
       </c>
     </row>
     <row r="36" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A36" s="54"/>
+      <c r="A36" s="56"/>
       <c r="B36" s="12">
         <v>0.41666666666666702</v>
       </c>
@@ -7360,7 +7398,7 @@
       </c>
     </row>
     <row r="37" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A37" s="54"/>
+      <c r="A37" s="56"/>
       <c r="B37" s="12">
         <v>0.45833333333333298</v>
       </c>
@@ -7408,7 +7446,7 @@
       </c>
     </row>
     <row r="38" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A38" s="54"/>
+      <c r="A38" s="56"/>
       <c r="B38" s="12">
         <v>0.5</v>
       </c>
@@ -7456,7 +7494,7 @@
       </c>
     </row>
     <row r="39" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A39" s="54"/>
+      <c r="A39" s="56"/>
       <c r="B39" s="12">
         <v>0.54166666666666696</v>
       </c>
@@ -7504,7 +7542,7 @@
       </c>
     </row>
     <row r="40" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A40" s="54"/>
+      <c r="A40" s="56"/>
       <c r="B40" s="12">
         <v>0.58333333333333304</v>
       </c>
@@ -7552,7 +7590,7 @@
       </c>
     </row>
     <row r="41" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A41" s="54"/>
+      <c r="A41" s="56"/>
       <c r="B41" s="12">
         <v>0.625</v>
       </c>
@@ -7600,7 +7638,7 @@
       </c>
     </row>
     <row r="42" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A42" s="54"/>
+      <c r="A42" s="56"/>
       <c r="B42" s="12">
         <v>0.66666666666666696</v>
       </c>
@@ -7648,7 +7686,7 @@
       </c>
     </row>
     <row r="43" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A43" s="54"/>
+      <c r="A43" s="56"/>
       <c r="B43" s="12">
         <v>0.70833333333333304</v>
       </c>
@@ -7696,7 +7734,7 @@
       </c>
     </row>
     <row r="44" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A44" s="54"/>
+      <c r="A44" s="56"/>
       <c r="B44" s="12">
         <v>0.75</v>
       </c>
@@ -7744,7 +7782,7 @@
       </c>
     </row>
     <row r="45" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A45" s="54"/>
+      <c r="A45" s="56"/>
       <c r="B45" s="12">
         <v>0.79166666666666696</v>
       </c>
@@ -7792,7 +7830,7 @@
       </c>
     </row>
     <row r="46" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A46" s="54"/>
+      <c r="A46" s="56"/>
       <c r="B46" s="12">
         <v>0.83333333333333304</v>
       </c>
@@ -7840,7 +7878,7 @@
       </c>
     </row>
     <row r="47" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A47" s="54"/>
+      <c r="A47" s="56"/>
       <c r="B47" s="12">
         <v>0.875</v>
       </c>
@@ -7888,7 +7926,7 @@
       </c>
     </row>
     <row r="48" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A48" s="54"/>
+      <c r="A48" s="56"/>
       <c r="B48" s="12">
         <v>0.91666666666666696</v>
       </c>
@@ -7936,7 +7974,7 @@
       </c>
     </row>
     <row r="49" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A49" s="54"/>
+      <c r="A49" s="56"/>
       <c r="B49" s="12">
         <v>0.95833333333333304</v>
       </c>
@@ -7984,7 +8022,7 @@
       </c>
     </row>
     <row r="50" spans="1:16" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="55"/>
+      <c r="A50" s="57"/>
       <c r="B50" s="13">
         <v>0.999999999999999</v>
       </c>
@@ -8032,7 +8070,7 @@
       </c>
     </row>
     <row r="51" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A51" s="56" t="s">
+      <c r="A51" s="58" t="s">
         <v>19</v>
       </c>
       <c r="B51" s="11">
@@ -8082,7 +8120,7 @@
       </c>
     </row>
     <row r="52" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A52" s="57"/>
+      <c r="A52" s="59"/>
       <c r="B52" s="12">
         <v>8.3333333333333301E-2</v>
       </c>
@@ -8130,7 +8168,7 @@
       </c>
     </row>
     <row r="53" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A53" s="57"/>
+      <c r="A53" s="59"/>
       <c r="B53" s="12">
         <v>0.125</v>
       </c>
@@ -8178,7 +8216,7 @@
       </c>
     </row>
     <row r="54" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A54" s="57"/>
+      <c r="A54" s="59"/>
       <c r="B54" s="12">
         <v>0.16666666666666699</v>
       </c>
@@ -8226,7 +8264,7 @@
       </c>
     </row>
     <row r="55" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A55" s="57"/>
+      <c r="A55" s="59"/>
       <c r="B55" s="12">
         <v>0.20833333333333301</v>
       </c>
@@ -8274,7 +8312,7 @@
       </c>
     </row>
     <row r="56" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A56" s="57"/>
+      <c r="A56" s="59"/>
       <c r="B56" s="12">
         <v>0.25</v>
       </c>
@@ -8322,7 +8360,7 @@
       </c>
     </row>
     <row r="57" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A57" s="57"/>
+      <c r="A57" s="59"/>
       <c r="B57" s="12">
         <v>0.29166666666666702</v>
       </c>
@@ -8370,7 +8408,7 @@
       </c>
     </row>
     <row r="58" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A58" s="57"/>
+      <c r="A58" s="59"/>
       <c r="B58" s="12">
         <v>0.33333333333333298</v>
       </c>
@@ -8418,7 +8456,7 @@
       </c>
     </row>
     <row r="59" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A59" s="57"/>
+      <c r="A59" s="59"/>
       <c r="B59" s="12">
         <v>0.375</v>
       </c>
@@ -8466,7 +8504,7 @@
       </c>
     </row>
     <row r="60" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A60" s="57"/>
+      <c r="A60" s="59"/>
       <c r="B60" s="12">
         <v>0.41666666666666702</v>
       </c>
@@ -8514,7 +8552,7 @@
       </c>
     </row>
     <row r="61" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A61" s="57"/>
+      <c r="A61" s="59"/>
       <c r="B61" s="12">
         <v>0.45833333333333298</v>
       </c>
@@ -8562,7 +8600,7 @@
       </c>
     </row>
     <row r="62" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A62" s="57"/>
+      <c r="A62" s="59"/>
       <c r="B62" s="12">
         <v>0.5</v>
       </c>
@@ -8610,7 +8648,7 @@
       </c>
     </row>
     <row r="63" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A63" s="57"/>
+      <c r="A63" s="59"/>
       <c r="B63" s="12">
         <v>0.54166666666666696</v>
       </c>
@@ -8658,7 +8696,7 @@
       </c>
     </row>
     <row r="64" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A64" s="57"/>
+      <c r="A64" s="59"/>
       <c r="B64" s="12">
         <v>0.58333333333333304</v>
       </c>
@@ -8706,7 +8744,7 @@
       </c>
     </row>
     <row r="65" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A65" s="57"/>
+      <c r="A65" s="59"/>
       <c r="B65" s="12">
         <v>0.625</v>
       </c>
@@ -8754,7 +8792,7 @@
       </c>
     </row>
     <row r="66" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A66" s="57"/>
+      <c r="A66" s="59"/>
       <c r="B66" s="12">
         <v>0.66666666666666696</v>
       </c>
@@ -8802,7 +8840,7 @@
       </c>
     </row>
     <row r="67" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A67" s="57"/>
+      <c r="A67" s="59"/>
       <c r="B67" s="12">
         <v>0.70833333333333304</v>
       </c>
@@ -8850,7 +8888,7 @@
       </c>
     </row>
     <row r="68" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A68" s="57"/>
+      <c r="A68" s="59"/>
       <c r="B68" s="12">
         <v>0.75</v>
       </c>
@@ -8898,7 +8936,7 @@
       </c>
     </row>
     <row r="69" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A69" s="57"/>
+      <c r="A69" s="59"/>
       <c r="B69" s="12">
         <v>0.79166666666666696</v>
       </c>
@@ -8946,7 +8984,7 @@
       </c>
     </row>
     <row r="70" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A70" s="57"/>
+      <c r="A70" s="59"/>
       <c r="B70" s="12">
         <v>0.83333333333333304</v>
       </c>
@@ -8994,7 +9032,7 @@
       </c>
     </row>
     <row r="71" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A71" s="57"/>
+      <c r="A71" s="59"/>
       <c r="B71" s="12">
         <v>0.875</v>
       </c>
@@ -9042,7 +9080,7 @@
       </c>
     </row>
     <row r="72" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A72" s="57"/>
+      <c r="A72" s="59"/>
       <c r="B72" s="12">
         <v>0.91666666666666696</v>
       </c>
@@ -9090,7 +9128,7 @@
       </c>
     </row>
     <row r="73" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A73" s="57"/>
+      <c r="A73" s="59"/>
       <c r="B73" s="12">
         <v>0.95833333333333304</v>
       </c>
@@ -9138,7 +9176,7 @@
       </c>
     </row>
     <row r="74" spans="1:16" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A74" s="58"/>
+      <c r="A74" s="60"/>
       <c r="B74" s="13">
         <v>0.999999999999999</v>
       </c>

</xml_diff>

<commit_message>
DHW calc in options in schedule
</commit_message>
<xml_diff>
--- a/eureca_ubem/Input/Schedules.xlsx
+++ b/eureca_ubem/Input/Schedules.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pratenr82256\Desktop\eureca-ubem\eureca_ubem\Input\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pratenr82256\Desktop\EUReCA\eureca_ubem\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5259458A-BD73-4BD7-8350-FBE0F10AC239}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55AC51ED-826A-4649-A9BE-779ED0E989B3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13950" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{102ADA3B-B81C-C94C-911C-48E8DF6FFDE7}"/>
+    <workbookView xWindow="14880" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{102ADA3B-B81C-C94C-911C-48E8DF6FFDE7}"/>
   </bookViews>
   <sheets>
     <sheet name="GeneralData" sheetId="10" r:id="rId1"/>
@@ -1277,7 +1277,7 @@
   <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:H8"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1480,11 +1480,11 @@
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G3:G105" xr:uid="{8D8140ED-8C4A-489F-8C7E-0BC81CB30031}">
-      <formula1>"Schedule,UNI-TS 11300-2"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H3:H1048576" xr:uid="{B24BD31C-DC54-4FED-B50C-B59BE5740BCD}">
       <formula1>"Schedule,Italian Residential Building Stock"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G3:G1048576" xr:uid="{B232E48A-8C69-4274-8B96-E2B211405633}">
+      <formula1>"Schedule,UNI-TS 11300-2,DHW calc"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>